<commit_message>
Implemented timeseries to supim file, demand file next
</commit_message>
<xml_diff>
--- a/Input/urbs_intertemporal_2050/2024.xlsx
+++ b/Input/urbs_intertemporal_2050/2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerald\Desktop\urbs-test\urbs\Input\urbs_intertemporal_2050\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerald\Desktop\urbsextension\Input\urbs_intertemporal_2050\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0D5EE2-B049-4A17-BE55-F92FBD5700FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B030B8-778C-41F6-AB6E-650FB1021AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="796" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="796" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="11" r:id="rId1"/>
@@ -2376,16 +2376,7 @@
     <cellStyle name="Zelle überprüfen 4" xfId="214" xr:uid="{00000000-0005-0000-0000-000092010000}"/>
     <cellStyle name="Zelle überprüfen 5" xfId="215" xr:uid="{00000000-0005-0000-0000-000093010000}"/>
   </cellStyles>
-  <dxfs count="25">
-    <dxf>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="24">
     <dxf>
       <border>
         <top style="thin">
@@ -3002,10 +2993,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D3"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -3055,6 +3046,160 @@
         <v>0.3</v>
       </c>
       <c r="D3" s="61">
+        <v>0.20699999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="5">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="C4">
+        <v>0.3</v>
+      </c>
+      <c r="D4" s="61">
+        <v>0.20699999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="C5">
+        <v>0.3</v>
+      </c>
+      <c r="D5" s="61">
+        <v>0.20699999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="5">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="C6">
+        <v>0.3</v>
+      </c>
+      <c r="D6" s="61">
+        <v>0.20699999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="5">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="C7">
+        <v>0.3</v>
+      </c>
+      <c r="D7" s="61">
+        <v>0.20699999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="5">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="C8">
+        <v>0.3</v>
+      </c>
+      <c r="D8" s="61">
+        <v>0.20699999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="5">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="C9">
+        <v>0.3</v>
+      </c>
+      <c r="D9" s="61">
+        <v>0.20699999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="5">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="C10">
+        <v>0.3</v>
+      </c>
+      <c r="D10" s="61">
+        <v>0.20699999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="5">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="C11">
+        <v>0.3</v>
+      </c>
+      <c r="D11" s="61">
+        <v>0.20699999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="5">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="C12">
+        <v>0.3</v>
+      </c>
+      <c r="D12" s="61">
+        <v>0.20699999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="5">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="C13">
+        <v>0.3</v>
+      </c>
+      <c r="D13" s="61">
+        <v>0.20699999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="5">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="C14">
+        <v>0.3</v>
+      </c>
+      <c r="D14" s="61">
         <v>0.20699999999999999</v>
       </c>
     </row>
@@ -3433,7 +3578,7 @@
   <autoFilter ref="B1:F6" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="B10:B11">
-    <cfRule type="expression" dxfId="24" priority="1">
+    <cfRule type="expression" dxfId="23" priority="1">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3454,7 +3599,7 @@
   </sheetPr>
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -4091,52 +4236,47 @@
   <autoFilter ref="A1:N1" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="A2:A13">
-    <cfRule type="expression" dxfId="23" priority="7">
+    <cfRule type="expression" dxfId="22" priority="7">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1 A2:E3 G2:XFD3 A4:XFD5 A6:E6 G6:XFD6">
-    <cfRule type="expression" dxfId="22" priority="9">
+    <cfRule type="expression" dxfId="21" priority="9">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B5">
-    <cfRule type="expression" dxfId="21" priority="8">
+    <cfRule type="expression" dxfId="20" priority="8">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:B10 B12:B13">
-    <cfRule type="expression" dxfId="20" priority="3">
+  <conditionalFormatting sqref="B7:B13">
+    <cfRule type="expression" dxfId="19" priority="1">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="19" priority="2">
+    <cfRule type="expression" dxfId="18" priority="2">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D13 P11:XFD19 A19 A20:XFD1048576">
-    <cfRule type="expression" dxfId="18" priority="10">
+    <cfRule type="expression" dxfId="17" priority="10">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E13">
-    <cfRule type="expression" dxfId="17" priority="5">
+    <cfRule type="expression" dxfId="16" priority="5">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="expression" dxfId="16" priority="4">
+    <cfRule type="expression" dxfId="15" priority="4">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:K4">
-    <cfRule type="expression" dxfId="15" priority="6">
-      <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="14" priority="6">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4754,32 +4894,32 @@
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <conditionalFormatting sqref="A1:XFD6 A7:C8 E7:XFD8 A9:XFD9 A10:C11 E10:XFD11 A12:XFD16 A17:C19 E17:XFD19 A20:XFD23 F24:XFD32 A33:XFD1048576">
-    <cfRule type="expression" dxfId="14" priority="29">
+    <cfRule type="expression" dxfId="13" priority="29">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:C31">
-    <cfRule type="expression" dxfId="13" priority="15">
+    <cfRule type="expression" dxfId="12" priority="15">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32:D32">
-    <cfRule type="expression" dxfId="12" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:E2">
-    <cfRule type="expression" dxfId="11" priority="36">
+    <cfRule type="expression" dxfId="10" priority="36">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:E24 A24:A32 D27:E27 D30:E30">
-    <cfRule type="expression" dxfId="10" priority="16">
+    <cfRule type="expression" dxfId="9" priority="16">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D23">
-    <cfRule type="expression" dxfId="9" priority="23">
+    <cfRule type="expression" dxfId="8" priority="23">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4880,7 +5020,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="8">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
     <cfRule type="dataBar" priority="9">
@@ -4923,7 +5063,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="5">
+    <cfRule type="expression" dxfId="6" priority="5">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
     <cfRule type="dataBar" priority="6">
@@ -5078,7 +5218,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25:E26">
-    <cfRule type="expression" dxfId="6" priority="14">
+    <cfRule type="expression" dxfId="5" priority="14">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5097,7 +5237,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28:E29">
-    <cfRule type="expression" dxfId="5" priority="12">
+    <cfRule type="expression" dxfId="4" priority="12">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5116,7 +5256,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31:E32">
-    <cfRule type="expression" dxfId="4" priority="10">
+    <cfRule type="expression" dxfId="3" priority="10">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5583,7 +5723,7 @@
   </sheetData>
   <autoFilter ref="A1:N1" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
   <conditionalFormatting sqref="M1">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5924,12 +6064,12 @@
   <autoFilter ref="A1:U1" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="A2:A4">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6045,10 +6185,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A1:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -6059,7 +6199,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
@@ -6079,7 +6219,95 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2516000000</v>
+        <v>209666667</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="5">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>209666667</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>209666667</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="5">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>209666667</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="5">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>209666667</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="5">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>209666667</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="5">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>209666667</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="5">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>209666667</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="5">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>209666667</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="5">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>209666667</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="5">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>209666667</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="5">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>209666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TODO fix lr scripts no longer working
</commit_message>
<xml_diff>
--- a/Input/urbs_intertemporal_2050/2024.xlsx
+++ b/Input/urbs_intertemporal_2050/2024.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerald\Desktop\urbsextension\Input\urbs_intertemporal_2050\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxoi\GitHub\urbs-extension\Input\urbs_intertemporal_2050\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B030B8-778C-41F6-AB6E-650FB1021AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CFD752-FD4C-4128-83B4-D2ABB4D8BB82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="796" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="796" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="11" r:id="rId1"/>
@@ -388,12 +388,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="45">
     <font>
@@ -1441,11 +1441,11 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1619,11 +1619,11 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
@@ -1652,11 +1652,11 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
@@ -1685,11 +1685,11 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
@@ -1728,20 +1728,20 @@
     <xf numFmtId="0" fontId="1" fillId="22" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1782,7 +1782,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1812,8 +1812,8 @@
     <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="25" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="2"/>
     </xf>
@@ -1823,7 +1823,7 @@
     <xf numFmtId="2" fontId="0" fillId="25" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="2"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="25" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="25" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="2"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1832,7 +1832,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" indent="2"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1845,7 +1845,7 @@
       <alignment horizontal="right" indent="2"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="24" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1909,7 +1909,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="68" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="69" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="69" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="69" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="69" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="69" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -1926,7 +1926,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="66" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2902,12 +2902,12 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="32" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" style="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="74.85546875" style="32" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="32"/>
+    <col min="1" max="1" width="14.109375" style="32" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" style="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="74.88671875" style="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="11.44140625" style="32"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2943,7 +2943,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="45">
+    <row r="4" spans="1:3" ht="43.2">
       <c r="A4" s="33" t="s">
         <v>61</v>
       </c>
@@ -2965,7 +2965,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30">
+    <row r="6" spans="1:3" ht="28.8">
       <c r="A6" s="33" t="s">
         <v>72</v>
       </c>
@@ -2996,15 +2996,15 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="2"/>
-    <col min="2" max="2" width="15.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="2"/>
+    <col min="1" max="1" width="11.44140625" style="2"/>
+    <col min="2" max="2" width="15.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="15" customFormat="1">
@@ -3226,9 +3226,9 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="16384" width="11.42578125" style="2"/>
+    <col min="1" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="15" customFormat="1">
@@ -3259,7 +3259,7 @@
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
@@ -3291,9 +3291,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3332,14 +3332,14 @@
       <selection activeCell="D6" sqref="D6:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="3" customWidth="1"/>
-    <col min="4" max="5" width="10.7109375" style="9" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="3"/>
+    <col min="1" max="1" width="10.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="3" customWidth="1"/>
+    <col min="4" max="5" width="10.6640625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.44140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" customFormat="1">
@@ -3599,26 +3599,26 @@
   </sheetPr>
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="10.7109375" style="20" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" style="20" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" style="20" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="10.6640625" style="20" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" style="20" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" style="20" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="3" customWidth="1"/>
     <col min="9" max="9" width="24" style="20" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" style="20" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="22" customWidth="1"/>
-    <col min="12" max="12" width="16.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.42578125" style="3"/>
+    <col min="10" max="10" width="10.6640625" style="20" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" style="22" customWidth="1"/>
+    <col min="12" max="12" width="16.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5546875" style="3" customWidth="1"/>
+    <col min="14" max="14" width="14.88671875" style="23" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.44140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" customFormat="1">
@@ -4311,14 +4311,14 @@
       <selection activeCell="A24" sqref="A24:E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="21" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" style="21" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="3"/>
+    <col min="1" max="1" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" style="21" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" style="21" customWidth="1"/>
+    <col min="6" max="16384" width="11.44140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" customFormat="1">
@@ -5651,20 +5651,20 @@
       <selection activeCell="A2" sqref="A2:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.7109375" style="21" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="20" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="23" customWidth="1"/>
-    <col min="10" max="13" width="10.7109375" style="20" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.6640625" style="21" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="20" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" style="23" customWidth="1"/>
+    <col min="10" max="13" width="10.6640625" style="20" customWidth="1"/>
+    <col min="14" max="14" width="14.88671875" style="23" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -5757,28 +5757,28 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="10.7109375" style="23" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.6640625" style="23" customWidth="1"/>
+    <col min="12" max="12" width="12.44140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.109375" style="23" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" style="20" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.7109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.42578125" style="23" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="12.140625" style="23" customWidth="1"/>
-    <col min="20" max="20" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.7109375" style="23" customWidth="1"/>
-    <col min="22" max="22" width="12.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.42578125" style="3"/>
+    <col min="15" max="15" width="11.6640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.44140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="12.109375" style="23" customWidth="1"/>
+    <col min="20" max="20" width="14.88671875" style="23" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.6640625" style="23" customWidth="1"/>
+    <col min="22" max="22" width="12.109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11.44140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -6111,13 +6111,13 @@
       <selection activeCell="A2" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" style="35" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6187,15 +6187,15 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A1:B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="2"/>
-    <col min="2" max="2" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="11.42578125" style="2"/>
+    <col min="1" max="1" width="11.44140625" style="2"/>
+    <col min="2" max="2" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">

</xml_diff>

<commit_message>
ruff formatted each files.
</commit_message>
<xml_diff>
--- a/Input/urbs_intertemporal_2050/2024.xlsx
+++ b/Input/urbs_intertemporal_2050/2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxoi\GitHub\urbs-extension\Input\urbs_intertemporal_2050\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CFD752-FD4C-4128-83B4-D2ABB4D8BB82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30F0F07-0B7B-4A65-A57D-93C6EA9B4155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="796" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="67080" yWindow="-1935" windowWidth="29040" windowHeight="17520" tabRatio="796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="11" r:id="rId1"/>
@@ -2898,8 +2898,8 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -3599,7 +3599,7 @@
   </sheetPr>
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added LNG. TODO Limit Piped Gas in Scenarios.py propably
</commit_message>
<xml_diff>
--- a/Input/urbs_intertemporal_2050/2024.xlsx
+++ b/Input/urbs_intertemporal_2050/2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxoi\GitHub\urbs-extension\Input\urbs_intertemporal_2050\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30F0F07-0B7B-4A65-A57D-93C6EA9B4155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76BB514-2993-4040-835B-1ECE6C7642B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67080" yWindow="-1935" windowWidth="29040" windowHeight="17520" tabRatio="796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-5445" windowWidth="38640" windowHeight="21120" tabRatio="796" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="11" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="112">
   <si>
     <t>t</t>
   </si>
@@ -381,6 +381,15 @@
   </si>
   <si>
     <t>Gas Plant (CCGT) CCUS</t>
+  </si>
+  <si>
+    <t>Piped Gas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LNG </t>
+  </si>
+  <si>
+    <t>Gas Plant (CCGT) LNG</t>
   </si>
 </sst>
 </file>
@@ -2376,7 +2385,34 @@
     <cellStyle name="Zelle überprüfen 4" xfId="214" xr:uid="{00000000-0005-0000-0000-000092010000}"/>
     <cellStyle name="Zelle überprüfen 5" xfId="215" xr:uid="{00000000-0005-0000-0000-000093010000}"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="27">
+    <dxf>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <border>
         <top style="thin">
@@ -2898,7 +2934,7 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -3326,10 +3362,10 @@
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:D11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -3465,7 +3501,7 @@
         <v>5</v>
       </c>
       <c r="D6">
-        <v>0.6</v>
+        <v>8.64</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>28</v>
@@ -3479,13 +3515,13 @@
         <v>99</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>6</v>
+        <v>109</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D7">
-        <v>1.75</v>
+        <v>22.68</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>28</v>
@@ -3525,7 +3561,7 @@
         <v>5</v>
       </c>
       <c r="D9">
-        <v>5.2</v>
+        <v>67.680000000000007</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>28</v>
@@ -3545,7 +3581,7 @@
         <v>5</v>
       </c>
       <c r="D10">
-        <v>0.47199999999999998</v>
+        <v>6.12</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>28</v>
@@ -3565,20 +3601,40 @@
         <v>5</v>
       </c>
       <c r="D11">
-        <v>0.5</v>
+        <v>6.48</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>28</v>
       </c>
       <c r="F11" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>23.62</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="8" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="B1:F6" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <phoneticPr fontId="0" type="noConversion"/>
-  <conditionalFormatting sqref="B10:B11">
-    <cfRule type="expression" dxfId="23" priority="1">
+  <conditionalFormatting sqref="B10:B12">
+    <cfRule type="expression" dxfId="26" priority="1">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3597,10 +3653,10 @@
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -4232,51 +4288,103 @@
         <v>#N/A</v>
       </c>
     </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" s="60" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="51">
+        <v>0</v>
+      </c>
+      <c r="D14" s="20">
+        <v>9</v>
+      </c>
+      <c r="E14" s="20">
+        <v>0</v>
+      </c>
+      <c r="F14" s="64">
+        <v>999999</v>
+      </c>
+      <c r="G14" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="54">
+        <v>0.25</v>
+      </c>
+      <c r="I14" s="55">
+        <v>802808.92800000007</v>
+      </c>
+      <c r="J14" s="55">
+        <v>16725.186000000002</v>
+      </c>
+      <c r="K14" s="56">
+        <v>2.6</v>
+      </c>
+      <c r="L14" s="57">
+        <v>0</v>
+      </c>
+      <c r="M14" s="42">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="N14" s="56">
+        <v>25</v>
+      </c>
+      <c r="O14" s="28" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:N1" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <phoneticPr fontId="0" type="noConversion"/>
-  <conditionalFormatting sqref="A2:A13">
-    <cfRule type="expression" dxfId="22" priority="7">
+  <conditionalFormatting sqref="A2:A14">
+    <cfRule type="expression" dxfId="6" priority="8">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1 A2:E3 G2:XFD3 A4:XFD5 A6:E6 G6:XFD6">
-    <cfRule type="expression" dxfId="21" priority="9">
+    <cfRule type="expression" dxfId="25" priority="10">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B5">
-    <cfRule type="expression" dxfId="20" priority="8">
+    <cfRule type="expression" dxfId="24" priority="9">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:B13">
-    <cfRule type="expression" dxfId="19" priority="1">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="18" priority="2">
+    <cfRule type="expression" dxfId="23" priority="3">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D13 P11:XFD19 A19 A20:XFD1048576">
-    <cfRule type="expression" dxfId="17" priority="10">
+  <conditionalFormatting sqref="P11:XFD19 A19 A20:XFD1048576 D3:D14">
+    <cfRule type="expression" dxfId="4" priority="11">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E13">
-    <cfRule type="expression" dxfId="16" priority="5">
+  <conditionalFormatting sqref="E2:E14">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="expression" dxfId="15" priority="4">
+    <cfRule type="expression" dxfId="22" priority="5">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:K4">
-    <cfRule type="expression" dxfId="14" priority="6">
+    <cfRule type="expression" dxfId="21" priority="7">
+      <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4305,10 +4413,10 @@
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:E32"/>
+      <selection activeCell="A33" sqref="A33:E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -4467,7 +4575,7 @@
         <v>91</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>6</v>
+        <v>109</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>40</v>
@@ -4891,40 +4999,93 @@
         <v>#N/A</v>
       </c>
     </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="60" t="s">
+        <v>111</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" s="24">
+        <v>1</v>
+      </c>
+      <c r="E33" s="24">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="60" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="E34" s="24" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="60" t="s">
+        <v>111</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="24">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="E35" s="24">
+        <f>D35*E33</f>
+        <v>0.24599999999999997</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
-  <conditionalFormatting sqref="A1:XFD6 A7:C8 E7:XFD8 A9:XFD9 A10:C11 E10:XFD11 A12:XFD16 A17:C19 E17:XFD19 A20:XFD23 F24:XFD32 A33:XFD1048576">
-    <cfRule type="expression" dxfId="13" priority="29">
+  <conditionalFormatting sqref="A1:XFD6 A7:C8 E7:XFD8 A9 A10:C11 E10:XFD11 A12:XFD16 A17:C19 E17:XFD19 A20:XFD23 F24:XFD32 A36:XFD1048576 C9:XFD9 A33 E34:XFD35 C33:XFD33 A34:C35">
+    <cfRule type="expression" dxfId="20" priority="34">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:C31">
-    <cfRule type="expression" dxfId="12" priority="15">
+    <cfRule type="expression" dxfId="19" priority="20">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32:D32">
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="18" priority="7">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:E2">
-    <cfRule type="expression" dxfId="10" priority="36">
+    <cfRule type="expression" dxfId="17" priority="41">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:E24 A24:A32 D27:E27 D30:E30">
-    <cfRule type="expression" dxfId="9" priority="16">
+    <cfRule type="expression" dxfId="16" priority="21">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D23">
-    <cfRule type="expression" dxfId="8" priority="23">
+    <cfRule type="expression" dxfId="15" priority="28">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="dataBar" priority="28">
+    <cfRule type="dataBar" priority="33">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -4938,7 +5099,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D11">
-    <cfRule type="dataBar" priority="26">
+    <cfRule type="dataBar" priority="31">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -4952,7 +5113,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:D14 D2:E6 D9:E9 E7:E8 E10:E11">
-    <cfRule type="dataBar" priority="35">
+    <cfRule type="dataBar" priority="40">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -4966,7 +5127,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17 D19">
-    <cfRule type="dataBar" priority="24">
+    <cfRule type="dataBar" priority="29">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -4980,7 +5141,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="dataBar" priority="22">
+    <cfRule type="dataBar" priority="27">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -4994,7 +5155,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24">
-    <cfRule type="dataBar" priority="18">
+    <cfRule type="dataBar" priority="23">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -5008,7 +5169,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26">
-    <cfRule type="dataBar" priority="7">
+    <cfRule type="dataBar" priority="12">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -5020,10 +5181,10 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="14" priority="13">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
-    <cfRule type="dataBar" priority="9">
+    <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -5037,7 +5198,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="dataBar" priority="17">
+    <cfRule type="dataBar" priority="22">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -5051,7 +5212,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29">
-    <cfRule type="dataBar" priority="4">
+    <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -5063,10 +5224,10 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="13" priority="10">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
-    <cfRule type="dataBar" priority="6">
+    <cfRule type="dataBar" priority="11">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -5080,7 +5241,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32">
-    <cfRule type="dataBar" priority="1">
+    <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -5092,7 +5253,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="dataBar" priority="3">
+    <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -5106,7 +5267,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15:E16 D2:D23">
-    <cfRule type="dataBar" priority="37">
+    <cfRule type="dataBar" priority="42">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -5120,7 +5281,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20:E21">
-    <cfRule type="dataBar" priority="31">
+    <cfRule type="dataBar" priority="36">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -5134,7 +5295,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22:E23">
-    <cfRule type="dataBar" priority="30">
+    <cfRule type="dataBar" priority="35">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -5148,7 +5309,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30:E30 E31">
-    <cfRule type="dataBar" priority="19">
+    <cfRule type="dataBar" priority="24">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -5161,8 +5322,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D33:E1048576 D1:E1">
-    <cfRule type="dataBar" priority="56">
+  <conditionalFormatting sqref="D36:E1048576 D1:E1">
+    <cfRule type="dataBar" priority="61">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -5176,7 +5337,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:E14">
-    <cfRule type="dataBar" priority="34">
+    <cfRule type="dataBar" priority="39">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -5190,7 +5351,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17:E19">
-    <cfRule type="dataBar" priority="32">
+    <cfRule type="dataBar" priority="37">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -5204,7 +5365,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24:E26">
-    <cfRule type="dataBar" priority="21">
+    <cfRule type="dataBar" priority="26">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -5218,12 +5379,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25:E26">
-    <cfRule type="expression" dxfId="5" priority="14">
+    <cfRule type="expression" dxfId="12" priority="19">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E27:E28">
-    <cfRule type="dataBar" priority="20">
+    <cfRule type="dataBar" priority="25">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -5237,12 +5398,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28:E29">
-    <cfRule type="expression" dxfId="4" priority="12">
+    <cfRule type="expression" dxfId="11" priority="17">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="dataBar" priority="13">
+    <cfRule type="dataBar" priority="18">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -5256,12 +5417,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31:E32">
-    <cfRule type="expression" dxfId="3" priority="10">
+    <cfRule type="expression" dxfId="10" priority="15">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="dataBar" priority="11">
+    <cfRule type="dataBar" priority="16">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -5272,6 +5433,58 @@
           <x14:id>{A7C290DA-E617-4412-A5C5-3335857A068B}</x14:id>
         </ext>
       </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33:D35">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34:D35">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="2"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{565012B0-F520-423C-81F4-0556E4C75B40}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33:E33 E34:E35">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="2"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{05321CB7-284A-4FA6-BF65-78097A8972CB}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33:D35">
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="2"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{28824AAA-F1F2-4A7D-928D-3858A69D3F02}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B33">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -5542,7 +5755,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D33:E1048576 D1:E1</xm:sqref>
+          <xm:sqref>D36:E1048576 D1:E1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{98CA02A6-D84B-4B8F-8EE0-BCA3C3E37146}">
@@ -5634,6 +5847,51 @@
           </x14:cfRule>
           <xm:sqref>E32</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{565012B0-F520-423C-81F4-0556E4C75B40}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D34:D35</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{05321CB7-284A-4FA6-BF65-78097A8972CB}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D33:E33 E34:E35</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{28824AAA-F1F2-4A7D-928D-3858A69D3F02}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D33:D35</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>
@@ -5723,7 +5981,7 @@
   </sheetData>
   <autoFilter ref="A1:N1" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
   <conditionalFormatting sqref="M1">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="9" priority="1">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6064,12 +6322,12 @@
   <autoFilter ref="A1:U1" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="A2:A4">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added LNG, next step limit piped gas supply and further adapt Inputs
</commit_message>
<xml_diff>
--- a/Input/urbs_intertemporal_2050/2024.xlsx
+++ b/Input/urbs_intertemporal_2050/2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxoi\GitHub\urbs-extension\Input\urbs_intertemporal_2050\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76BB514-2993-4040-835B-1ECE6C7642B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74B4A82-514D-4C0C-8AC3-CB7648646BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5445" windowWidth="38640" windowHeight="21120" tabRatio="796" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="67080" yWindow="-1935" windowWidth="29040" windowHeight="17520" tabRatio="796" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="11" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="111">
   <si>
     <t>t</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>Stock</t>
-  </si>
-  <si>
-    <t>Gas</t>
   </si>
   <si>
     <t>price</t>
@@ -2385,16 +2382,7 @@
     <cellStyle name="Zelle überprüfen 4" xfId="214" xr:uid="{00000000-0005-0000-0000-000092010000}"/>
     <cellStyle name="Zelle überprüfen 5" xfId="215" xr:uid="{00000000-0005-0000-0000-000093010000}"/>
   </cellStyles>
-  <dxfs count="27">
-    <dxf>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="26">
     <dxf>
       <border>
         <top style="thin">
@@ -2948,68 +2936,68 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="31" t="s">
         <v>62</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="37">
         <v>2024</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="37">
         <v>0.03</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="43.2">
       <c r="A4" s="33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="63">
         <v>505160000</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="28.8">
       <c r="A6" s="33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" s="62">
         <v>4426360000</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -3048,13 +3036,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="D1" s="14" t="s">
         <v>102</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3272,10 +3260,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>80</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -3302,10 +3290,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>104</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -3334,15 +3322,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B2" s="7">
         <v>280000000</v>
@@ -3380,30 +3368,30 @@
   <sheetData>
     <row r="1" spans="1:6" customFormat="1">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>8</v>
-      </c>
       <c r="F1" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>3</v>
@@ -3423,10 +3411,10 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>3</v>
@@ -3446,7 +3434,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>1</v>
@@ -3469,10 +3457,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>4</v>
@@ -3492,10 +3480,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>5</v>
@@ -3504,18 +3492,18 @@
         <v>8.64</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>5</v>
@@ -3524,38 +3512,38 @@
         <v>22.68</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="D8">
         <v>65</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>5</v>
@@ -3564,18 +3552,18 @@
         <v>67.680000000000007</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>5</v>
@@ -3584,18 +3572,18 @@
         <v>6.12</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>5</v>
@@ -3604,18 +3592,18 @@
         <v>6.48</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>5</v>
@@ -3624,17 +3612,17 @@
         <v>23.62</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="B1:F6" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="B10:B12">
-    <cfRule type="expression" dxfId="26" priority="1">
+    <cfRule type="expression" dxfId="25" priority="1">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3655,8 +3643,8 @@
   </sheetPr>
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -3679,57 +3667,57 @@
   <sheetData>
     <row r="1" spans="1:15" customFormat="1">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="F1" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="H1" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="I1" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="19" t="s">
+      <c r="M1" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="M1" s="16" t="s">
+      <c r="N1" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="16" t="s">
-        <v>17</v>
-      </c>
       <c r="O1" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C2" s="50">
         <v>195300</v>
@@ -3744,7 +3732,7 @@
         <v>379885</v>
       </c>
       <c r="G2" s="53" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H2" s="54">
         <v>0</v>
@@ -3773,10 +3761,10 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B3" s="49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C3" s="51">
         <v>18880</v>
@@ -3791,7 +3779,7 @@
         <v>240293.44961681674</v>
       </c>
       <c r="G3" s="53" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H3" s="54">
         <v>0</v>
@@ -3820,10 +3808,10 @@
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" s="49" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C4" s="51">
         <v>46710</v>
@@ -3838,7 +3826,7 @@
         <v>46710</v>
       </c>
       <c r="G4" s="53" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H4" s="54">
         <v>0</v>
@@ -3867,10 +3855,10 @@
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B5" s="49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C5" s="51">
         <v>59840</v>
@@ -3885,7 +3873,7 @@
         <v>59840</v>
       </c>
       <c r="G5" s="53" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H5" s="54">
         <v>0</v>
@@ -3914,10 +3902,10 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B6" s="49" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C6" s="51">
         <v>53560</v>
@@ -3932,7 +3920,7 @@
         <v>999999</v>
       </c>
       <c r="G6" s="53" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H6" s="54">
         <v>0.5</v>
@@ -3961,10 +3949,10 @@
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C7" s="51">
         <v>43590</v>
@@ -3979,7 +3967,7 @@
         <v>999999</v>
       </c>
       <c r="G7" s="53" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H7" s="54">
         <v>0.65</v>
@@ -4008,10 +3996,10 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B8" s="49" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C8" s="51">
         <v>188900</v>
@@ -4026,7 +4014,7 @@
         <v>999999</v>
       </c>
       <c r="G8" s="53" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H8" s="54">
         <v>0.25</v>
@@ -4055,10 +4043,10 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C9" s="51">
         <v>94200</v>
@@ -4073,7 +4061,7 @@
         <v>94200</v>
       </c>
       <c r="G9" s="53" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H9" s="54">
         <v>0</v>
@@ -4102,10 +4090,10 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C10" s="51">
         <v>20420</v>
@@ -4120,7 +4108,7 @@
         <v>999999999999</v>
       </c>
       <c r="G10" s="53" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H10" s="54">
         <v>0</v>
@@ -4149,10 +4137,10 @@
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B11" s="49" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C11" s="51">
         <v>0</v>
@@ -4167,7 +4155,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="53" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H11" s="54">
         <v>0.5</v>
@@ -4196,10 +4184,10 @@
     </row>
     <row r="12" spans="1:15">
       <c r="A12" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B12" s="49" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C12" s="51">
         <v>0</v>
@@ -4214,7 +4202,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="53" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H12" s="54">
         <v>0.65</v>
@@ -4243,10 +4231,10 @@
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B13" s="49" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C13" s="65">
         <v>0</v>
@@ -4261,7 +4249,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="53" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H13" s="54">
         <v>0.25</v>
@@ -4290,10 +4278,10 @@
     </row>
     <row r="14" spans="1:15">
       <c r="A14" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B14" s="60" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C14" s="51">
         <v>0</v>
@@ -4308,7 +4296,7 @@
         <v>999999</v>
       </c>
       <c r="G14" s="53" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H14" s="54">
         <v>0.25</v>
@@ -4339,52 +4327,47 @@
   <autoFilter ref="A1:N1" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="A2:A14">
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="24" priority="8">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1 A2:E3 G2:XFD3 A4:XFD5 A6:E6 G6:XFD6">
-    <cfRule type="expression" dxfId="25" priority="10">
+    <cfRule type="expression" dxfId="23" priority="10">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B5">
-    <cfRule type="expression" dxfId="24" priority="9">
+    <cfRule type="expression" dxfId="22" priority="9">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:B13">
-    <cfRule type="expression" dxfId="5" priority="2">
+  <conditionalFormatting sqref="B7:B14">
+    <cfRule type="expression" dxfId="21" priority="1">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="23" priority="3">
+    <cfRule type="expression" dxfId="20" priority="3">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P11:XFD19 A19 A20:XFD1048576 D3:D14">
-    <cfRule type="expression" dxfId="4" priority="11">
+  <conditionalFormatting sqref="D3:D14 P11:XFD19 A19 A20:XFD1048576">
+    <cfRule type="expression" dxfId="19" priority="11">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E14">
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="18" priority="6">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="expression" dxfId="22" priority="5">
+    <cfRule type="expression" dxfId="17" priority="5">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:K4">
-    <cfRule type="expression" dxfId="21" priority="7">
-      <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B14">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="16" priority="7">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4415,8 +4398,8 @@
   </sheetPr>
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:E35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -4431,30 +4414,30 @@
   <sheetData>
     <row r="1" spans="1:5" customFormat="1">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="60" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" s="24">
         <v>1</v>
@@ -4466,13 +4449,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="60" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="24">
         <v>1</v>
@@ -4484,13 +4467,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="60" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" s="24">
         <v>1</v>
@@ -4502,13 +4485,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="60" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D5" s="24">
         <v>1</v>
@@ -4520,13 +4503,13 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="60" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="24">
         <v>1</v>
@@ -4537,13 +4520,13 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="60" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D7" s="24">
         <v>0.41</v>
@@ -4555,13 +4538,13 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="60" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8" s="24">
         <v>0.36299999999999999</v>
@@ -4572,13 +4555,13 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="60" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9" s="24">
         <v>1</v>
@@ -4589,13 +4572,13 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="60" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="24">
         <v>0.6</v>
@@ -4607,13 +4590,13 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="60" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="24">
         <v>0.20499999999999999</v>
@@ -4625,13 +4608,13 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="60" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12" s="24">
         <v>1</v>
@@ -4643,13 +4626,13 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="60" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" s="24">
         <v>0.35</v>
@@ -4661,13 +4644,13 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="60" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D14" s="24">
         <v>0</v>
@@ -4679,13 +4662,13 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="60" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="24">
         <v>1</v>
@@ -4697,13 +4680,13 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="60" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D16" s="24">
         <v>0.38</v>
@@ -4715,13 +4698,13 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="60" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" s="24">
         <v>1</v>
@@ -4732,13 +4715,13 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="60" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" s="24">
         <v>0.45</v>
@@ -4750,13 +4733,13 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="60" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D19" s="24">
         <v>0.34179999999999999</v>
@@ -4768,13 +4751,13 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="60" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D20" s="24">
         <v>1</v>
@@ -4786,13 +4769,13 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="60" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D21" s="24">
         <v>1</v>
@@ -4804,13 +4787,13 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="60" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D22" s="24">
         <v>1</v>
@@ -4822,13 +4805,13 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="60" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23" s="24">
         <v>1</v>
@@ -4840,13 +4823,13 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="60" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D24" s="24">
         <v>1</v>
@@ -4858,13 +4841,13 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="60" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D25" s="66">
         <v>0.36</v>
@@ -4876,13 +4859,13 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="60" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D26" s="67">
         <v>3.4180000000000002E-2</v>
@@ -4894,13 +4877,13 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="60" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D27" s="24">
         <v>1</v>
@@ -4912,13 +4895,13 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="60" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D28" s="66">
         <v>0.32</v>
@@ -4930,13 +4913,13 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="60" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D29" s="67">
         <v>3.6299999999999999E-2</v>
@@ -4948,13 +4931,13 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="60" t="s">
+        <v>107</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>6</v>
-      </c>
       <c r="C30" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D30" s="24">
         <v>1</v>
@@ -4965,13 +4948,13 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="60" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D31" s="66">
         <v>0.4</v>
@@ -4983,13 +4966,13 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="60" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D32" s="67">
         <v>2.0500000000000001E-2</v>
@@ -5001,13 +4984,13 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="60" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D33" s="24">
         <v>1</v>
@@ -5018,13 +5001,13 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="60" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D34" s="24">
         <v>0.6</v>
@@ -5036,13 +5019,13 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="60" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D35" s="24">
         <v>0.20499999999999999</v>
@@ -5054,33 +5037,38 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
-  <conditionalFormatting sqref="A1:XFD6 A7:C8 E7:XFD8 A9 A10:C11 E10:XFD11 A12:XFD16 A17:C19 E17:XFD19 A20:XFD23 F24:XFD32 A36:XFD1048576 C9:XFD9 A33 E34:XFD35 C33:XFD33 A34:C35">
-    <cfRule type="expression" dxfId="20" priority="34">
+  <conditionalFormatting sqref="A1:XFD6 A7:C8 E7:XFD8 A9 C9:XFD9 A10:C11 E10:XFD11 A12:XFD16 A17:C19 E17:XFD19 A20:XFD23 F24:XFD32 A34:C35 E34:XFD35 A36:XFD1048576">
+    <cfRule type="expression" dxfId="15" priority="34">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B25:C31">
-    <cfRule type="expression" dxfId="19" priority="20">
+  <conditionalFormatting sqref="B25:C29 B31:C31 C30">
+    <cfRule type="expression" dxfId="14" priority="20">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32:D32">
-    <cfRule type="expression" dxfId="18" priority="7">
+    <cfRule type="expression" dxfId="13" priority="7">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:E2">
-    <cfRule type="expression" dxfId="17" priority="41">
+    <cfRule type="expression" dxfId="12" priority="41">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B24:E24 A24:A32 D27:E27 D30:E30">
-    <cfRule type="expression" dxfId="16" priority="21">
+  <conditionalFormatting sqref="B24:E24 A24:A33 D27:E27 D30:E30">
+    <cfRule type="expression" dxfId="11" priority="21">
+      <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B33:XFD33">
+    <cfRule type="expression" dxfId="10" priority="1">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D23">
-    <cfRule type="expression" dxfId="15" priority="28">
+    <cfRule type="expression" dxfId="9" priority="28">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5181,7 +5169,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="13">
+    <cfRule type="expression" dxfId="8" priority="13">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
     <cfRule type="dataBar" priority="14">
@@ -5224,7 +5212,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="10">
+    <cfRule type="expression" dxfId="7" priority="10">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
     <cfRule type="dataBar" priority="11">
@@ -5262,6 +5250,37 @@
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{B2637DB6-30FE-4484-B8A4-D99048727AA5}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33:D35">
+    <cfRule type="expression" dxfId="6" priority="2">
+      <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
+    </cfRule>
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="2"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{28824AAA-F1F2-4A7D-928D-3858A69D3F02}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34:D35">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="2"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{565012B0-F520-423C-81F4-0556E4C75B40}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -5318,6 +5337,20 @@
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{69715B00-4721-4DC7-BD2B-D23473816C64}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33:E33 E34:E35">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="2"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{05321CB7-284A-4FA6-BF65-78097A8972CB}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -5379,7 +5412,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25:E26">
-    <cfRule type="expression" dxfId="12" priority="19">
+    <cfRule type="expression" dxfId="5" priority="19">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5398,7 +5431,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28:E29">
-    <cfRule type="expression" dxfId="11" priority="17">
+    <cfRule type="expression" dxfId="4" priority="17">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5417,7 +5450,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31:E32">
-    <cfRule type="expression" dxfId="10" priority="15">
+    <cfRule type="expression" dxfId="3" priority="15">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5433,58 +5466,6 @@
           <x14:id>{A7C290DA-E617-4412-A5C5-3335857A068B}</x14:id>
         </ext>
       </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D33:D35">
-    <cfRule type="expression" dxfId="2" priority="2">
-      <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D34:D35">
-    <cfRule type="dataBar" priority="3">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="2"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{565012B0-F520-423C-81F4-0556E4C75B40}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D33:E33 E34:E35">
-    <cfRule type="dataBar" priority="4">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="2"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{05321CB7-284A-4FA6-BF65-78097A8972CB}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D33:D35">
-    <cfRule type="dataBar" priority="5">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="2"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{28824AAA-F1F2-4A7D-928D-3858A69D3F02}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B33">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -5683,6 +5664,36 @@
           <xm:sqref>D32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{28824AAA-F1F2-4A7D-928D-3858A69D3F02}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D33:D35</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{565012B0-F520-423C-81F4-0556E4C75B40}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D34:D35</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{F00EA992-7704-4FFF-9390-9F67541314D3}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
@@ -5741,6 +5752,21 @@
             </x14:dataBar>
           </x14:cfRule>
           <xm:sqref>D30:E30 E31</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{05321CB7-284A-4FA6-BF65-78097A8972CB}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D33:E33 E34:E35</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{0F5F82D7-D9D8-496A-8067-873F84F07A41}">
@@ -5847,51 +5873,6 @@
           </x14:cfRule>
           <xm:sqref>E32</xm:sqref>
         </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{565012B0-F520-423C-81F4-0556E4C75B40}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>2</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>D34:D35</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{05321CB7-284A-4FA6-BF65-78097A8972CB}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>2</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>D33:E33 E34:E35</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{28824AAA-F1F2-4A7D-928D-3858A69D3F02}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>2</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>D33:D35</xm:sqref>
-        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>
@@ -5927,61 +5908,61 @@
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E1" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="G1" s="17" t="s">
+      <c r="H1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="I1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="J1" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="16" t="s">
+      <c r="N1" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="16" t="s">
-        <v>17</v>
-      </c>
       <c r="O1" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="P1" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="Q1" s="16" t="s">
         <v>78</v>
-      </c>
-      <c r="Q1" s="16" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:N1" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
   <conditionalFormatting sqref="M1">
-    <cfRule type="expression" dxfId="9" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6041,84 +6022,84 @@
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="C1" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D1" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="H1" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="I1" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="17" t="s">
+      <c r="J1" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="K1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="16" t="s">
-        <v>25</v>
-      </c>
       <c r="L1" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="N1" s="17" t="s">
+      <c r="O1" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="P1" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="Q1" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" s="16" t="s">
+      <c r="R1" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="S1" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="U1" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="S1" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T1" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="U1" s="16" t="s">
-        <v>35</v>
-      </c>
       <c r="V1" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W1" s="36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:23">
       <c r="A2" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C2" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="39">
         <v>0</v>
@@ -6127,7 +6108,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G2" s="39">
         <v>0</v>
@@ -6136,7 +6117,7 @@
         <v>0</v>
       </c>
       <c r="I2" s="39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J2" s="44">
         <v>0.66</v>
@@ -6181,13 +6162,13 @@
     </row>
     <row r="3" spans="1:23">
       <c r="A3" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B3" s="41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" s="39">
         <v>0</v>
@@ -6196,7 +6177,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G3" s="39">
         <v>0</v>
@@ -6205,7 +6186,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J3" s="45">
         <v>0.9</v>
@@ -6251,13 +6232,13 @@
     </row>
     <row r="4" spans="1:23">
       <c r="A4" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" s="39">
         <v>0</v>
@@ -6266,7 +6247,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G4" s="39">
         <v>0</v>
@@ -6275,7 +6256,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J4" s="48">
         <v>0.86</v>
@@ -6322,12 +6303,12 @@
   <autoFilter ref="A1:U1" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="A2:A4">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S1">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6381,25 +6362,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="17" t="s">
+      <c r="F1" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="G1" s="17" t="s">
         <v>53</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -6461,7 +6442,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:2">

</xml_diff>

<commit_message>
deleted offshore and onshore from urbs classic inputs
</commit_message>
<xml_diff>
--- a/Input/urbs_intertemporal_2050/2024.xlsx
+++ b/Input/urbs_intertemporal_2050/2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxoi\GitHub\urbs-extension\Input\urbs_intertemporal_2050\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74B4A82-514D-4C0C-8AC3-CB7648646BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6507CB46-1A04-4473-A680-0002A32E6BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67080" yWindow="-1935" windowWidth="29040" windowHeight="17520" tabRatio="796" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-5445" windowWidth="38640" windowHeight="21120" tabRatio="796" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="11" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <sheet name="TimeVarEff" sheetId="15" r:id="rId12"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Commodity!$B$1:$F$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Commodity!$B$1:$F$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">DSM!$A$1:$G$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3">Process!$A$1:$N$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Process-Commodity'!$A$1:$E$1</definedName>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="105">
   <si>
     <t>t</t>
   </si>
@@ -308,12 +308,6 @@
     <t>Li-ion battery</t>
   </si>
   <si>
-    <t>Wind (onshore)</t>
-  </si>
-  <si>
-    <t>Wind (offshore)</t>
-  </si>
-  <si>
     <t>Hydro (run-of-river)</t>
   </si>
   <si>
@@ -335,12 +329,6 @@
     <t>Biomass Plant</t>
   </si>
   <si>
-    <t>WindOff</t>
-  </si>
-  <si>
-    <t>WindOn</t>
-  </si>
-  <si>
     <t>Biomass</t>
   </si>
   <si>
@@ -354,12 +342,6 @@
   </si>
   <si>
     <t>EU27.Elec</t>
-  </si>
-  <si>
-    <t>EU27.WindOff</t>
-  </si>
-  <si>
-    <t>EU27.WindOn</t>
   </si>
   <si>
     <t>EU27.Hydro</t>
@@ -1783,7 +1765,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1908,7 +1890,6 @@
     <xf numFmtId="0" fontId="0" fillId="24" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="25" fillId="66" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="25" fillId="66" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="25" fillId="67" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="68" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2382,43 +2363,7 @@
     <cellStyle name="Zelle überprüfen 4" xfId="214" xr:uid="{00000000-0005-0000-0000-000092010000}"/>
     <cellStyle name="Zelle überprüfen 5" xfId="215" xr:uid="{00000000-0005-0000-0000-000093010000}"/>
   </cellStyles>
-  <dxfs count="26">
-    <dxf>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="22">
     <dxf>
       <border>
         <top style="thin">
@@ -2971,7 +2916,7 @@
       <c r="A4" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="63">
+      <c r="B4" s="62">
         <v>505160000</v>
       </c>
       <c r="C4" s="29" t="s">
@@ -2993,7 +2938,7 @@
       <c r="A6" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="B6" s="62">
+      <c r="B6" s="61">
         <v>4426360000</v>
       </c>
       <c r="C6" s="29" t="s">
@@ -3001,7 +2946,7 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="B7" s="62"/>
+      <c r="B7" s="61"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -3017,223 +2962,131 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="2"/>
-    <col min="2" max="2" width="15.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="11.44140625" style="2"/>
+    <col min="1" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="15" customFormat="1">
+    <row r="1" spans="1:2" s="15" customFormat="1">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="5">
         <v>0</v>
       </c>
       <c r="B2" s="27">
         <v>0</v>
       </c>
-      <c r="C2" s="27">
-        <v>0</v>
-      </c>
-      <c r="D2" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="C3">
-        <v>0.3</v>
-      </c>
-      <c r="D3" s="61">
+      <c r="B3" s="60">
         <v>0.20699999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:2">
       <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="C4">
-        <v>0.3</v>
-      </c>
-      <c r="D4" s="61">
+      <c r="B4" s="60">
         <v>0.20699999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:2">
       <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="C5">
-        <v>0.3</v>
-      </c>
-      <c r="D5" s="61">
+      <c r="B5" s="60">
         <v>0.20699999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:2">
       <c r="A6" s="5">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="C6">
-        <v>0.3</v>
-      </c>
-      <c r="D6" s="61">
+      <c r="B6" s="60">
         <v>0.20699999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:2">
       <c r="A7" s="5">
         <v>5</v>
       </c>
-      <c r="B7">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="C7">
-        <v>0.3</v>
-      </c>
-      <c r="D7" s="61">
+      <c r="B7" s="60">
         <v>0.20699999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:2">
       <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="C8">
-        <v>0.3</v>
-      </c>
-      <c r="D8" s="61">
+      <c r="B8" s="60">
         <v>0.20699999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:2">
       <c r="A9" s="5">
         <v>7</v>
       </c>
-      <c r="B9">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="C9">
-        <v>0.3</v>
-      </c>
-      <c r="D9" s="61">
+      <c r="B9" s="60">
         <v>0.20699999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:2">
       <c r="A10" s="5">
         <v>8</v>
       </c>
-      <c r="B10">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="C10">
-        <v>0.3</v>
-      </c>
-      <c r="D10" s="61">
+      <c r="B10" s="60">
         <v>0.20699999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:2">
       <c r="A11" s="5">
         <v>9</v>
       </c>
-      <c r="B11">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="C11">
-        <v>0.3</v>
-      </c>
-      <c r="D11" s="61">
+      <c r="B11" s="60">
         <v>0.20699999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:2">
       <c r="A12" s="5">
         <v>10</v>
       </c>
-      <c r="B12">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="C12">
-        <v>0.3</v>
-      </c>
-      <c r="D12" s="61">
+      <c r="B12" s="60">
         <v>0.20699999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:2">
       <c r="A13" s="5">
         <v>11</v>
       </c>
-      <c r="B13">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="C13">
-        <v>0.3</v>
-      </c>
-      <c r="D13" s="61">
+      <c r="B13" s="60">
         <v>0.20699999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:2">
       <c r="A14" s="5">
         <v>12</v>
       </c>
-      <c r="B14">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="C14">
-        <v>0.3</v>
-      </c>
-      <c r="D14" s="61">
+      <c r="B14" s="60">
         <v>0.20699999999999999</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
-  <dataValidations count="3">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Capacity factor Wind" prompt="Normalized capacity factor (maximum value 1) of wind power. Determines EPrIn of processes with input commodity Wind." sqref="B1" xr:uid="{95B70FA2-D121-47BA-B169-E55C0A467113}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Capacity factor Hydro" prompt="Normalized capacity factor (maximum value 1) of hydro power. Determines EPrIn of processes with input commodity Hydro." sqref="C1" xr:uid="{A326FD59-F9D1-4CB7-A642-E7C2042D9719}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="B2:C2" xr:uid="{11057201-016F-428D-AFA9-0DCAEDA5A9E2}"/>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3290,10 +3143,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -3330,7 +3183,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B2" s="7">
         <v>280000000</v>
@@ -3350,10 +3203,10 @@
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A3" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -3388,10 +3241,10 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>93</v>
+        <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>3</v>
@@ -3411,13 +3264,13 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>94</v>
+        <v>35</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3" s="28" t="e">
         <f>NA()</f>
@@ -3434,82 +3287,76 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="28" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E4" s="28" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F4" s="28" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>8.64</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="28" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E5" s="28" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F5" s="28" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>22.68</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="D6">
-        <v>8.64</v>
+        <v>65</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D7">
-        <v>22.68</v>
+        <v>67.680000000000007</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>27</v>
@@ -3520,36 +3367,36 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>25</v>
+        <v>92</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="D8">
-        <v>65</v>
+        <v>6.12</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D9">
-        <v>67.680000000000007</v>
+        <v>6.48</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>27</v>
@@ -3560,16 +3407,16 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D10">
-        <v>6.12</v>
+        <v>23.62</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>27</v>
@@ -3578,51 +3425,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11">
-        <v>6.48</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12">
-        <v>23.62</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="B1:F6" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
+  <autoFilter ref="B1:F4" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <phoneticPr fontId="0" type="noConversion"/>
-  <conditionalFormatting sqref="B10:B12">
-    <cfRule type="expression" dxfId="25" priority="1">
+  <conditionalFormatting sqref="B8:B10">
+    <cfRule type="expression" dxfId="21" priority="1">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3641,10 +3448,10 @@
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+      <selection activeCell="A3" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -3714,46 +3521,46 @@
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B2" s="49" t="s">
         <v>84</v>
       </c>
       <c r="C2" s="50">
-        <v>195300</v>
+        <v>46710</v>
       </c>
       <c r="D2" s="20">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E2" s="20">
         <v>0</v>
       </c>
-      <c r="F2" s="64">
-        <v>379885</v>
-      </c>
-      <c r="G2" s="53" t="s">
+      <c r="F2" s="51">
+        <v>46710</v>
+      </c>
+      <c r="G2" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="54">
-        <v>0</v>
-      </c>
-      <c r="I2" s="55">
-        <v>1187151.4952</v>
-      </c>
-      <c r="J2" s="55">
-        <v>14639.04184</v>
-      </c>
-      <c r="K2" s="56">
-        <v>0</v>
-      </c>
-      <c r="L2" s="56">
+      <c r="H2" s="53">
+        <v>0</v>
+      </c>
+      <c r="I2" s="54">
+        <v>2731780.3800000004</v>
+      </c>
+      <c r="J2" s="54">
+        <v>9923.6103600000006</v>
+      </c>
+      <c r="K2" s="54">
+        <v>0</v>
+      </c>
+      <c r="L2" s="55">
         <v>0</v>
       </c>
       <c r="M2" s="42">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="N2" s="56">
-        <v>25</v>
+      <c r="N2" s="55">
+        <v>60</v>
       </c>
       <c r="O2" s="28" t="e">
         <v>#N/A</v>
@@ -3761,46 +3568,46 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B3" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="51">
-        <v>18880</v>
+      <c r="C3" s="50">
+        <v>59840</v>
       </c>
       <c r="D3" s="20">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E3" s="20">
         <v>0</v>
       </c>
-      <c r="F3" s="64">
-        <v>240293.44961681674</v>
-      </c>
-      <c r="G3" s="53" t="s">
+      <c r="F3" s="51">
+        <v>59840</v>
+      </c>
+      <c r="G3" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="54">
+      <c r="H3" s="53">
         <v>0</v>
       </c>
       <c r="I3" s="55">
-        <v>2204404.6215999997</v>
+        <v>3345037.2</v>
       </c>
       <c r="J3" s="55">
-        <v>41352.62184</v>
-      </c>
-      <c r="K3" s="56">
-        <v>0</v>
-      </c>
-      <c r="L3" s="56">
+        <v>28432.799999999999</v>
+      </c>
+      <c r="K3" s="55">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="L3" s="55">
         <v>0</v>
       </c>
       <c r="M3" s="42">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="N3" s="56">
-        <v>25</v>
+      <c r="N3" s="55">
+        <v>50</v>
       </c>
       <c r="O3" s="28" t="e">
         <v>#N/A</v>
@@ -3808,46 +3615,46 @@
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B4" s="49" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="51">
-        <v>46710</v>
+      <c r="C4" s="50">
+        <v>53560</v>
       </c>
       <c r="D4" s="20">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="E4" s="20">
         <v>0</v>
       </c>
-      <c r="F4" s="52">
-        <v>46710</v>
-      </c>
-      <c r="G4" s="53" t="s">
+      <c r="F4" s="63">
+        <v>999999</v>
+      </c>
+      <c r="G4" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="54">
-        <v>0</v>
-      </c>
-      <c r="I4" s="55">
-        <v>2731780.3800000004</v>
-      </c>
-      <c r="J4" s="55">
-        <v>9923.6103600000006</v>
-      </c>
-      <c r="K4" s="55">
-        <v>0</v>
-      </c>
-      <c r="L4" s="56">
+      <c r="H4" s="53">
+        <v>0.5</v>
+      </c>
+      <c r="I4" s="56">
+        <v>1784013.3447999998</v>
+      </c>
+      <c r="J4" s="57">
+        <v>28544.213516800002</v>
+      </c>
+      <c r="K4" s="54">
+        <v>2.7</v>
+      </c>
+      <c r="L4" s="55">
         <v>0</v>
       </c>
       <c r="M4" s="42">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="N4" s="56">
-        <v>60</v>
+      <c r="N4" s="55">
+        <v>40</v>
       </c>
       <c r="O4" s="28" t="e">
         <v>#N/A</v>
@@ -3855,46 +3662,46 @@
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B5" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="C5" s="51">
-        <v>59840</v>
+      <c r="C5" s="50">
+        <v>43590</v>
       </c>
       <c r="D5" s="20">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="E5" s="20">
         <v>0</v>
       </c>
-      <c r="F5" s="52">
-        <v>59840</v>
-      </c>
-      <c r="G5" s="53" t="s">
+      <c r="F5" s="63">
+        <v>999999</v>
+      </c>
+      <c r="G5" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="54">
-        <v>0</v>
-      </c>
-      <c r="I5" s="56">
-        <v>3345037.2</v>
-      </c>
-      <c r="J5" s="56">
-        <v>28432.799999999999</v>
-      </c>
-      <c r="K5" s="56">
-        <v>0.35699999999999998</v>
-      </c>
-      <c r="L5" s="56">
+      <c r="H5" s="53">
+        <v>0.65</v>
+      </c>
+      <c r="I5" s="54">
+        <v>2230016.6809999999</v>
+      </c>
+      <c r="J5" s="54">
+        <v>52182.390330800001</v>
+      </c>
+      <c r="K5" s="55">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="L5" s="55">
         <v>0</v>
       </c>
       <c r="M5" s="42">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="N5" s="56">
-        <v>50</v>
+      <c r="N5" s="55">
+        <v>40</v>
       </c>
       <c r="O5" s="28" t="e">
         <v>#N/A</v>
@@ -3902,37 +3709,37 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B6" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="51">
-        <v>53560</v>
+      <c r="C6" s="50">
+        <v>188900</v>
       </c>
       <c r="D6" s="20">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E6" s="20">
         <v>0</v>
       </c>
-      <c r="F6" s="64">
+      <c r="F6" s="63">
         <v>999999</v>
       </c>
-      <c r="G6" s="53" t="s">
+      <c r="G6" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="54">
-        <v>0.5</v>
-      </c>
-      <c r="I6" s="57">
-        <v>1784013.3447999998</v>
-      </c>
-      <c r="J6" s="58">
-        <v>28544.213516800002</v>
+      <c r="H6" s="53">
+        <v>0.25</v>
+      </c>
+      <c r="I6" s="54">
+        <v>802808.92800000007</v>
+      </c>
+      <c r="J6" s="54">
+        <v>16725.186000000002</v>
       </c>
       <c r="K6" s="55">
-        <v>2.7</v>
+        <v>2.6</v>
       </c>
       <c r="L6" s="56">
         <v>0</v>
@@ -3940,8 +3747,8 @@
       <c r="M6" s="42">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="N6" s="56">
-        <v>40</v>
+      <c r="N6" s="55">
+        <v>25</v>
       </c>
       <c r="O6" s="28" t="e">
         <v>#N/A</v>
@@ -3949,46 +3756,46 @@
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B7" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="51">
-        <v>43590</v>
+      <c r="C7" s="50">
+        <v>94200</v>
       </c>
       <c r="D7" s="20">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="E7" s="20">
         <v>0</v>
       </c>
-      <c r="F7" s="64">
-        <v>999999</v>
-      </c>
-      <c r="G7" s="53" t="s">
+      <c r="F7" s="50">
+        <v>94200</v>
+      </c>
+      <c r="G7" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="54">
-        <v>0.65</v>
-      </c>
-      <c r="I7" s="55">
-        <v>2230016.6809999999</v>
-      </c>
-      <c r="J7" s="55">
-        <v>52182.390330800001</v>
-      </c>
-      <c r="K7" s="56">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="L7" s="56">
+      <c r="H7" s="53">
+        <v>0</v>
+      </c>
+      <c r="I7" s="54">
+        <v>5909565.7200000007</v>
+      </c>
+      <c r="J7" s="57">
+        <v>133801.48800000001</v>
+      </c>
+      <c r="K7" s="54">
+        <v>7.1</v>
+      </c>
+      <c r="L7" s="55">
         <v>0</v>
       </c>
       <c r="M7" s="42">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="N7" s="56">
-        <v>40</v>
+      <c r="N7" s="55">
+        <v>60</v>
       </c>
       <c r="O7" s="28" t="e">
         <v>#N/A</v>
@@ -3996,45 +3803,45 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B8" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="51">
-        <v>188900</v>
+      <c r="C8" s="50">
+        <v>20420</v>
       </c>
       <c r="D8" s="20">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E8" s="20">
         <v>0</v>
       </c>
-      <c r="F8" s="64">
-        <v>999999</v>
-      </c>
-      <c r="G8" s="53" t="s">
+      <c r="F8" s="20">
+        <v>999999999999</v>
+      </c>
+      <c r="G8" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="54">
-        <v>0.25</v>
-      </c>
-      <c r="I8" s="55">
-        <v>802808.92800000007</v>
-      </c>
-      <c r="J8" s="55">
-        <v>16725.186000000002</v>
-      </c>
-      <c r="K8" s="56">
-        <v>2.6</v>
-      </c>
-      <c r="L8" s="57">
+      <c r="H8" s="53">
+        <v>0</v>
+      </c>
+      <c r="I8" s="58">
+        <v>5648000</v>
+      </c>
+      <c r="J8" s="58">
+        <v>0</v>
+      </c>
+      <c r="K8" s="58">
+        <v>44.2</v>
+      </c>
+      <c r="L8" s="55">
         <v>0</v>
       </c>
       <c r="M8" s="42">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="N8" s="56">
+      <c r="N8" s="55">
         <v>25</v>
       </c>
       <c r="O8" s="28" t="e">
@@ -4043,37 +3850,37 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" s="51">
-        <v>94200</v>
+        <v>99</v>
+      </c>
+      <c r="C9" s="50">
+        <v>0</v>
       </c>
       <c r="D9" s="20">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="E9" s="20">
         <v>0</v>
       </c>
-      <c r="F9" s="51">
-        <v>94200</v>
-      </c>
-      <c r="G9" s="53" t="s">
+      <c r="F9" s="50">
+        <v>0</v>
+      </c>
+      <c r="G9" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="54">
-        <v>0</v>
+      <c r="H9" s="53">
+        <v>0.5</v>
       </c>
       <c r="I9" s="55">
-        <v>5909565.7200000007</v>
-      </c>
-      <c r="J9" s="58">
-        <v>133801.48800000001</v>
+        <v>3791028.3572399998</v>
+      </c>
+      <c r="J9" s="55">
+        <v>84183.129702000006</v>
       </c>
       <c r="K9" s="55">
-        <v>7.1</v>
+        <v>6.75</v>
       </c>
       <c r="L9" s="56">
         <v>0</v>
@@ -4081,8 +3888,8 @@
       <c r="M9" s="42">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="N9" s="56">
-        <v>60</v>
+      <c r="N9" s="55">
+        <v>40</v>
       </c>
       <c r="O9" s="28" t="e">
         <v>#N/A</v>
@@ -4090,37 +3897,37 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>92</v>
-      </c>
-      <c r="C10" s="51">
-        <v>20420</v>
+        <v>100</v>
+      </c>
+      <c r="C10" s="50">
+        <v>0</v>
       </c>
       <c r="D10" s="20">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E10" s="20">
         <v>0</v>
       </c>
-      <c r="F10" s="20">
-        <v>999999999999</v>
-      </c>
-      <c r="G10" s="53" t="s">
+      <c r="F10" s="50">
+        <v>0</v>
+      </c>
+      <c r="G10" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="54">
-        <v>0</v>
-      </c>
-      <c r="I10" s="59">
-        <v>5648000</v>
-      </c>
-      <c r="J10" s="59">
-        <v>0</v>
-      </c>
-      <c r="K10" s="59">
-        <v>44.2</v>
+      <c r="H10" s="53">
+        <v>0.65</v>
+      </c>
+      <c r="I10" s="55">
+        <v>4014030.0248799999</v>
+      </c>
+      <c r="J10" s="55">
+        <v>76489.572146799997</v>
+      </c>
+      <c r="K10" s="55">
+        <v>6.96</v>
       </c>
       <c r="L10" s="56">
         <v>0</v>
@@ -4128,8 +3935,8 @@
       <c r="M10" s="42">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="N10" s="56">
-        <v>25</v>
+      <c r="N10" s="55">
+        <v>40</v>
       </c>
       <c r="O10" s="28" t="e">
         <v>#N/A</v>
@@ -4137,12 +3944,12 @@
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B11" s="49" t="s">
-        <v>105</v>
-      </c>
-      <c r="C11" s="51">
+        <v>101</v>
+      </c>
+      <c r="C11" s="64">
         <v>0</v>
       </c>
       <c r="D11" s="20">
@@ -4151,32 +3958,32 @@
       <c r="E11" s="20">
         <v>0</v>
       </c>
-      <c r="F11" s="51">
-        <v>0</v>
-      </c>
-      <c r="G11" s="53" t="s">
+      <c r="F11" s="50">
+        <v>0</v>
+      </c>
+      <c r="G11" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="54">
-        <v>0.5</v>
-      </c>
-      <c r="I11" s="56">
-        <v>3791028.3572399998</v>
-      </c>
-      <c r="J11" s="56">
-        <v>84183.129702000006</v>
-      </c>
-      <c r="K11" s="56">
-        <v>6.75</v>
-      </c>
-      <c r="L11" s="57">
+      <c r="H11" s="53">
+        <v>0.25</v>
+      </c>
+      <c r="I11" s="55">
+        <v>1951271.6999999997</v>
+      </c>
+      <c r="J11" s="55">
+        <v>45715.5</v>
+      </c>
+      <c r="K11" s="55">
+        <v>3.46</v>
+      </c>
+      <c r="L11" s="56">
         <v>0</v>
       </c>
       <c r="M11" s="42">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="N11" s="56">
-        <v>40</v>
+      <c r="N11" s="55">
+        <v>25</v>
       </c>
       <c r="O11" s="28" t="e">
         <v>#N/A</v>
@@ -4184,190 +3991,86 @@
     </row>
     <row r="12" spans="1:15">
       <c r="A12" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B12" s="49" t="s">
-        <v>106</v>
-      </c>
-      <c r="C12" s="51">
+        <v>94</v>
+      </c>
+      <c r="B12" s="59" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12" s="50">
         <v>0</v>
       </c>
       <c r="D12" s="20">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E12" s="20">
         <v>0</v>
       </c>
-      <c r="F12" s="51">
-        <v>0</v>
-      </c>
-      <c r="G12" s="53" t="s">
+      <c r="F12" s="63">
+        <v>999999</v>
+      </c>
+      <c r="G12" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="54">
-        <v>0.65</v>
-      </c>
-      <c r="I12" s="56">
-        <v>4014030.0248799999</v>
-      </c>
-      <c r="J12" s="56">
-        <v>76489.572146799997</v>
-      </c>
-      <c r="K12" s="56">
-        <v>6.96</v>
-      </c>
-      <c r="L12" s="57">
+      <c r="H12" s="53">
+        <v>0.25</v>
+      </c>
+      <c r="I12" s="54">
+        <v>802808.92800000007</v>
+      </c>
+      <c r="J12" s="54">
+        <v>16725.186000000002</v>
+      </c>
+      <c r="K12" s="55">
+        <v>2.6</v>
+      </c>
+      <c r="L12" s="56">
         <v>0</v>
       </c>
       <c r="M12" s="42">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="N12" s="56">
-        <v>40</v>
+      <c r="N12" s="55">
+        <v>25</v>
       </c>
       <c r="O12" s="28" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="A13" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B13" s="49" t="s">
-        <v>107</v>
-      </c>
-      <c r="C13" s="65">
-        <v>0</v>
-      </c>
-      <c r="D13" s="20">
-        <v>0</v>
-      </c>
-      <c r="E13" s="20">
-        <v>0</v>
-      </c>
-      <c r="F13" s="51">
-        <v>0</v>
-      </c>
-      <c r="G13" s="53" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" s="54">
-        <v>0.25</v>
-      </c>
-      <c r="I13" s="56">
-        <v>1951271.6999999997</v>
-      </c>
-      <c r="J13" s="56">
-        <v>45715.5</v>
-      </c>
-      <c r="K13" s="56">
-        <v>3.46</v>
-      </c>
-      <c r="L13" s="57">
-        <v>0</v>
-      </c>
-      <c r="M13" s="42">
-        <v>7.0999999999999994E-2</v>
-      </c>
-      <c r="N13" s="56">
-        <v>25</v>
-      </c>
-      <c r="O13" s="28" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="A14" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B14" s="60" t="s">
-        <v>110</v>
-      </c>
-      <c r="C14" s="51">
-        <v>0</v>
-      </c>
-      <c r="D14" s="20">
-        <v>9</v>
-      </c>
-      <c r="E14" s="20">
-        <v>0</v>
-      </c>
-      <c r="F14" s="64">
-        <v>999999</v>
-      </c>
-      <c r="G14" s="53" t="s">
-        <v>27</v>
-      </c>
-      <c r="H14" s="54">
-        <v>0.25</v>
-      </c>
-      <c r="I14" s="55">
-        <v>802808.92800000007</v>
-      </c>
-      <c r="J14" s="55">
-        <v>16725.186000000002</v>
-      </c>
-      <c r="K14" s="56">
-        <v>2.6</v>
-      </c>
-      <c r="L14" s="57">
-        <v>0</v>
-      </c>
-      <c r="M14" s="42">
-        <v>7.0999999999999994E-2</v>
-      </c>
-      <c r="N14" s="56">
-        <v>25</v>
-      </c>
-      <c r="O14" s="28" t="e">
         <v>#N/A</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:N1" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <phoneticPr fontId="0" type="noConversion"/>
-  <conditionalFormatting sqref="A2:A14">
-    <cfRule type="expression" dxfId="24" priority="8">
+  <conditionalFormatting sqref="A2:A12 B2:B3 D2:E12">
+    <cfRule type="expression" dxfId="20" priority="8">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD1 A2:E3 G2:XFD3 A4:XFD5 A6:E6 G6:XFD6">
-    <cfRule type="expression" dxfId="23" priority="10">
+  <conditionalFormatting sqref="A1:XFD3 A4:E4 G4:XFD4">
+    <cfRule type="expression" dxfId="19" priority="10">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B5">
-    <cfRule type="expression" dxfId="22" priority="9">
+  <conditionalFormatting sqref="B5:B12">
+    <cfRule type="expression" dxfId="18" priority="1">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:B14">
-    <cfRule type="expression" dxfId="21" priority="1">
+  <conditionalFormatting sqref="C11">
+    <cfRule type="expression" dxfId="17" priority="3">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="20" priority="3">
+  <conditionalFormatting sqref="P9:XFD17 A17 A18:XFD1048576">
+    <cfRule type="expression" dxfId="16" priority="11">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D14 P11:XFD19 A19 A20:XFD1048576">
-    <cfRule type="expression" dxfId="19" priority="11">
+  <conditionalFormatting sqref="F8">
+    <cfRule type="expression" dxfId="15" priority="5">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E14">
-    <cfRule type="expression" dxfId="18" priority="6">
-      <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F10">
-    <cfRule type="expression" dxfId="17" priority="5">
-      <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I4:K4">
-    <cfRule type="expression" dxfId="16" priority="7">
+  <conditionalFormatting sqref="I2:K2">
+    <cfRule type="expression" dxfId="14" priority="7">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4396,10 +4099,10 @@
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -4430,11 +4133,11 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="60" t="s">
-        <v>84</v>
+      <c r="A2" s="59" t="s">
+        <v>87</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>94</v>
+        <v>36</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>39</v>
@@ -4442,14 +4145,13 @@
       <c r="D2" s="24">
         <v>1</v>
       </c>
-      <c r="E2" s="24" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="E2" s="24">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="60" t="s">
-        <v>84</v>
+      <c r="A3" s="59" t="s">
+        <v>87</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>35</v>
@@ -4458,7 +4160,7 @@
         <v>40</v>
       </c>
       <c r="D3" s="24">
-        <v>1</v>
+        <v>0.41</v>
       </c>
       <c r="E3" s="24" t="e">
         <f>NA()</f>
@@ -4466,122 +4168,123 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="60" t="s">
-        <v>85</v>
+      <c r="A4" s="59" t="s">
+        <v>87</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>93</v>
+        <v>25</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="24">
+        <v>0.36299999999999999</v>
+      </c>
+      <c r="E4" s="24">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D5" s="24">
         <v>1</v>
       </c>
-      <c r="E4" s="24" t="e">
+      <c r="E5" s="24">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="E6" s="24" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="60" t="s">
-        <v>85</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="4" t="s">
+    <row r="7" spans="1:5">
+      <c r="A7" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D7" s="24">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="E7" s="24">
+        <f>D7*E5</f>
+        <v>0.24599999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="24">
         <v>1</v>
       </c>
-      <c r="E5" s="24" t="e">
+      <c r="E8" s="24" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="24">
-        <v>1</v>
-      </c>
-      <c r="E6" s="24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="B7" s="4" t="s">
+    <row r="9" spans="1:5">
+      <c r="A9" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="24">
-        <v>0.41</v>
-      </c>
-      <c r="E7" s="24" t="e">
+      <c r="D9" s="24">
+        <v>0.35</v>
+      </c>
+      <c r="E9" s="24" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="B8" s="4" t="s">
+    <row r="10" spans="1:5">
+      <c r="A10" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="24">
-        <v>0.36299999999999999</v>
-      </c>
-      <c r="E8" s="24">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="60" t="s">
-        <v>90</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="24">
-        <v>1</v>
-      </c>
-      <c r="E9" s="24">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="60" t="s">
-        <v>90</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>40</v>
       </c>
       <c r="D10" s="24">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="E10" s="24" t="e">
         <f>NA()</f>
@@ -4589,35 +4292,35 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="60" t="s">
-        <v>90</v>
+      <c r="A11" s="59" t="s">
+        <v>89</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>25</v>
+        <v>92</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="24">
+        <v>1</v>
+      </c>
+      <c r="E11" s="24" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="59" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="24">
-        <v>0.20499999999999999</v>
-      </c>
-      <c r="E11" s="24">
-        <f>D11*E9</f>
-        <v>0.24599999999999997</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="60" t="s">
-        <v>92</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="D12" s="24">
-        <v>1</v>
+        <v>0.38</v>
       </c>
       <c r="E12" s="24" t="e">
         <f>NA()</f>
@@ -4625,35 +4328,34 @@
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="60" t="s">
-        <v>92</v>
+      <c r="A13" s="59" t="s">
+        <v>86</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="24">
+        <v>1</v>
+      </c>
+      <c r="E13" s="24">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="59" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="24">
-        <v>0.35</v>
-      </c>
-      <c r="E13" s="24" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="60" t="s">
-        <v>92</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>40</v>
       </c>
       <c r="D14" s="24">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="E14" s="24" t="e">
         <f>NA()</f>
@@ -4661,35 +4363,35 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="60" t="s">
-        <v>91</v>
+      <c r="A15" s="59" t="s">
+        <v>86</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>96</v>
+        <v>25</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="24">
+        <v>0.34179999999999999</v>
+      </c>
+      <c r="E15" s="24">
+        <f>D15*E13</f>
+        <v>0.47851999999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="59" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D16" s="24">
         <v>1</v>
-      </c>
-      <c r="E15" s="24" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="60" t="s">
-        <v>91</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="24">
-        <v>0.38</v>
       </c>
       <c r="E16" s="24" t="e">
         <f>NA()</f>
@@ -4697,34 +4399,35 @@
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="60" t="s">
-        <v>88</v>
+      <c r="A17" s="59" t="s">
+        <v>84</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>97</v>
+        <v>35</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D17" s="24">
         <v>1</v>
       </c>
-      <c r="E17" s="24">
-        <v>1.4</v>
+      <c r="E17" s="24" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="60" t="s">
-        <v>88</v>
+      <c r="A18" s="59" t="s">
+        <v>85</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D18" s="24">
-        <v>0.45</v>
+        <v>1</v>
       </c>
       <c r="E18" s="24" t="e">
         <f>NA()</f>
@@ -4732,29 +4435,29 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="60" t="s">
-        <v>88</v>
+      <c r="A19" s="59" t="s">
+        <v>85</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>40</v>
       </c>
       <c r="D19" s="24">
-        <v>0.34179999999999999</v>
-      </c>
-      <c r="E19" s="24">
-        <f>D19*E17</f>
-        <v>0.47851999999999995</v>
+        <v>1</v>
+      </c>
+      <c r="E19" s="24" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="60" t="s">
-        <v>86</v>
+      <c r="A20" s="59" t="s">
+        <v>99</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>1</v>
+        <v>93</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>39</v>
@@ -4768,8 +4471,8 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="60" t="s">
-        <v>86</v>
+      <c r="A21" s="59" t="s">
+        <v>99</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>35</v>
@@ -4777,41 +4480,41 @@
       <c r="C21" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="24">
-        <v>1</v>
+      <c r="D21" s="65">
+        <v>0.36</v>
       </c>
       <c r="E21" s="24" t="e">
-        <f>NA()</f>
+        <f>D21*E19</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="60" t="s">
-        <v>87</v>
+      <c r="A22" s="59" t="s">
+        <v>99</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="66">
+        <v>3.4180000000000002E-2</v>
+      </c>
+      <c r="E22" s="24" t="e">
+        <f>D22*E20</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="59" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="D22" s="24">
-        <v>1</v>
-      </c>
-      <c r="E22" s="24" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="60" t="s">
-        <v>87</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="D23" s="24">
         <v>1</v>
@@ -4822,35 +4525,35 @@
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="60" t="s">
-        <v>105</v>
+      <c r="A24" s="59" t="s">
+        <v>100</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>97</v>
+        <v>35</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="24">
-        <v>1</v>
+        <v>40</v>
+      </c>
+      <c r="D24" s="65">
+        <v>0.32</v>
       </c>
       <c r="E24" s="24" t="e">
-        <f>NA()</f>
+        <f>D24*E21</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="60" t="s">
-        <v>105</v>
+      <c r="A25" s="59" t="s">
+        <v>100</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>40</v>
       </c>
       <c r="D25" s="66">
-        <v>0.36</v>
+        <v>3.6299999999999999E-2</v>
       </c>
       <c r="E25" s="24" t="e">
         <f>D25*E23</f>
@@ -4858,35 +4561,34 @@
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="60" t="s">
-        <v>105</v>
+      <c r="A26" s="59" t="s">
+        <v>101</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>25</v>
+        <v>102</v>
       </c>
       <c r="C26" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="24">
+        <v>1</v>
+      </c>
+      <c r="E26" s="24">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="59" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="67">
-        <v>3.4180000000000002E-2</v>
-      </c>
-      <c r="E26" s="24" t="e">
-        <f>D26*E24</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="60" t="s">
-        <v>106</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" s="24">
-        <v>1</v>
+      <c r="D27" s="65">
+        <v>0.4</v>
       </c>
       <c r="E27" s="24" t="e">
         <f>NA()</f>
@@ -4894,185 +4596,104 @@
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="60" t="s">
-        <v>106</v>
+      <c r="A28" s="59" t="s">
+        <v>101</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>40</v>
       </c>
       <c r="D28" s="66">
-        <v>0.32</v>
+        <v>2.0500000000000001E-2</v>
       </c>
       <c r="E28" s="24" t="e">
-        <f>D28*E25</f>
+        <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="60" t="s">
-        <v>106</v>
+      <c r="A29" s="59" t="s">
+        <v>104</v>
       </c>
       <c r="B29" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="24">
+        <v>1</v>
+      </c>
+      <c r="E29" s="24">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="59" t="s">
+        <v>104</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="E30" s="24" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="59" t="s">
+        <v>104</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D29" s="67">
-        <v>3.6299999999999999E-2</v>
-      </c>
-      <c r="E29" s="24" t="e">
-        <f>D29*E27</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D30" s="24">
-        <v>1</v>
-      </c>
-      <c r="E30" s="24">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D31" s="66">
-        <v>0.4</v>
-      </c>
-      <c r="E31" s="24" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D32" s="67">
-        <v>2.0500000000000001E-2</v>
-      </c>
-      <c r="E32" s="24" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="60" t="s">
-        <v>110</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D33" s="24">
-        <v>1</v>
-      </c>
-      <c r="E33" s="24">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="60" t="s">
-        <v>110</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D34" s="24">
-        <v>0.6</v>
-      </c>
-      <c r="E34" s="24" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="60" t="s">
-        <v>110</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D35" s="24">
+      <c r="D31" s="24">
         <v>0.20499999999999999</v>
       </c>
-      <c r="E35" s="24">
-        <f>D35*E33</f>
+      <c r="E31" s="24">
+        <f>D31*E29</f>
         <v>0.24599999999999997</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
-  <conditionalFormatting sqref="A1:XFD6 A7:C8 E7:XFD8 A9 C9:XFD9 A10:C11 E10:XFD11 A12:XFD16 A17:C19 E17:XFD19 A20:XFD23 F24:XFD32 A34:C35 E34:XFD35 A36:XFD1048576">
-    <cfRule type="expression" dxfId="15" priority="34">
+  <conditionalFormatting sqref="A3:C4 E3:XFD4 A5 C5:XFD5 A6:C7 E6:XFD7 A8:XFD12 A13:C15 E13:XFD15 A16:XFD19 F20:XFD28 A30:C31 E30:XFD31 A32:XFD1048576 A1:XFD2 D2:D19">
+    <cfRule type="expression" dxfId="13" priority="34">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B25:C29 B31:C31 C30">
-    <cfRule type="expression" dxfId="14" priority="20">
+  <conditionalFormatting sqref="B21:C25 C26:E26 B27:C27">
+    <cfRule type="expression" dxfId="12" priority="20">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B32:D32">
-    <cfRule type="expression" dxfId="13" priority="7">
+  <conditionalFormatting sqref="B28:D28">
+    <cfRule type="expression" dxfId="11" priority="7">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:E2">
-    <cfRule type="expression" dxfId="12" priority="41">
+  <conditionalFormatting sqref="B20:E20 A20:A29 D23:E23">
+    <cfRule type="expression" dxfId="10" priority="21">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B24:E24 A24:A33 D27:E27 D30:E30">
-    <cfRule type="expression" dxfId="11" priority="21">
+  <conditionalFormatting sqref="B29:XFD29">
+    <cfRule type="expression" dxfId="9" priority="1">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B33:XFD33">
-    <cfRule type="expression" dxfId="10" priority="1">
-      <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D23">
-    <cfRule type="expression" dxfId="9" priority="28">
-      <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
+  <conditionalFormatting sqref="D2:E2 D2:D19">
     <cfRule type="dataBar" priority="33">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5086,7 +4707,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D10:D11">
+  <conditionalFormatting sqref="D6:D7">
     <cfRule type="dataBar" priority="31">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5100,7 +4721,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D12:D14 D2:E6 D9:E9 E7:E8 E10:E11">
+  <conditionalFormatting sqref="D8:D10 D5:E5 E3:E4 E6:E7">
     <cfRule type="dataBar" priority="40">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5114,7 +4735,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D17 D19">
+  <conditionalFormatting sqref="D13 D15">
     <cfRule type="dataBar" priority="29">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5128,7 +4749,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D19">
+  <conditionalFormatting sqref="D15">
     <cfRule type="dataBar" priority="27">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5142,7 +4763,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D24">
+  <conditionalFormatting sqref="D20">
     <cfRule type="dataBar" priority="23">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5156,7 +4777,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D26">
+  <conditionalFormatting sqref="D22">
     <cfRule type="dataBar" priority="12">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5185,7 +4806,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D27">
+  <conditionalFormatting sqref="D23">
     <cfRule type="dataBar" priority="22">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5199,7 +4820,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D29">
+  <conditionalFormatting sqref="D25">
     <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5228,7 +4849,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
+  <conditionalFormatting sqref="D28">
     <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5254,7 +4875,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D33:D35">
+  <conditionalFormatting sqref="D29:D31">
     <cfRule type="expression" dxfId="6" priority="2">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
@@ -5271,7 +4892,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34:D35">
+  <conditionalFormatting sqref="D30:D31">
     <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5285,7 +4906,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D15:E16 D2:D23">
+  <conditionalFormatting sqref="D11:E12">
     <cfRule type="dataBar" priority="42">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5299,7 +4920,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D20:E21">
+  <conditionalFormatting sqref="D16:E17">
     <cfRule type="dataBar" priority="36">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5313,7 +4934,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D22:E23">
+  <conditionalFormatting sqref="D18:E19">
     <cfRule type="dataBar" priority="35">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5327,7 +4948,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D30:E30 E31">
+  <conditionalFormatting sqref="D26:E26 E27">
     <cfRule type="dataBar" priority="24">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5341,7 +4962,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D33:E33 E34:E35">
+  <conditionalFormatting sqref="D29:E29 E30:E31">
     <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5355,7 +4976,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36:E1048576 D1:E1">
+  <conditionalFormatting sqref="D32:E1048576 D1:E1">
     <cfRule type="dataBar" priority="61">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5369,7 +4990,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E12:E14">
+  <conditionalFormatting sqref="E8:E10">
     <cfRule type="dataBar" priority="39">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5383,7 +5004,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E17:E19">
+  <conditionalFormatting sqref="E13:E15">
     <cfRule type="dataBar" priority="37">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5397,7 +5018,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E24:E26">
+  <conditionalFormatting sqref="E20:E22">
     <cfRule type="dataBar" priority="26">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5411,12 +5032,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E25:E26">
+  <conditionalFormatting sqref="E21:E22">
     <cfRule type="expression" dxfId="5" priority="19">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E27:E28">
+  <conditionalFormatting sqref="E23:E24">
     <cfRule type="dataBar" priority="25">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5430,12 +5051,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E28:E29">
+  <conditionalFormatting sqref="E24:E25">
     <cfRule type="expression" dxfId="4" priority="17">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
+  <conditionalFormatting sqref="E25">
     <cfRule type="dataBar" priority="18">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5449,12 +5070,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E31:E32">
+  <conditionalFormatting sqref="E27:E28">
     <cfRule type="expression" dxfId="3" priority="15">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E32">
+  <conditionalFormatting sqref="E28">
     <cfRule type="dataBar" priority="16">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5490,7 +5111,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D8</xm:sqref>
+          <xm:sqref>D2:E2 D2:D19</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C0F1B5C9-46CC-4068-A4A5-2BE845D64618}">
@@ -5505,7 +5126,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D10:D11</xm:sqref>
+          <xm:sqref>D6:D7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{4EFF1923-5632-46D2-BEE4-19792B834F3E}">
@@ -5520,7 +5141,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D12:D14 D2:E6 D9:E9 E7:E8 E10:E11</xm:sqref>
+          <xm:sqref>D8:D10 D5:E5 E3:E4 E6:E7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{FD70C683-63D2-4AF7-9844-0053BE6DF679}">
@@ -5535,7 +5156,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D17 D19</xm:sqref>
+          <xm:sqref>D13 D15</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C12684E9-C44A-443A-881A-7ED428CB9718}">
@@ -5550,7 +5171,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D19</xm:sqref>
+          <xm:sqref>D15</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{DF85B3E7-6D24-4702-AB47-0D47F71538F8}">
@@ -5565,7 +5186,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D24</xm:sqref>
+          <xm:sqref>D20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{F7E4DC53-D7B5-4205-8087-340EC79B984A}">
@@ -5592,7 +5213,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D26</xm:sqref>
+          <xm:sqref>D22</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{638DB081-4439-4940-9AE3-880EB91DD8D4}">
@@ -5607,7 +5228,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D27</xm:sqref>
+          <xm:sqref>D23</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{4FA8C8CC-9E06-4AAF-9D36-B69E2717DF17}">
@@ -5634,7 +5255,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D29</xm:sqref>
+          <xm:sqref>D25</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6B773CE8-FE95-4E79-8BA2-717E6DDC4252}">
@@ -5661,7 +5282,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D32</xm:sqref>
+          <xm:sqref>D28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{28824AAA-F1F2-4A7D-928D-3858A69D3F02}">
@@ -5676,7 +5297,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D33:D35</xm:sqref>
+          <xm:sqref>D29:D31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{565012B0-F520-423C-81F4-0556E4C75B40}">
@@ -5691,7 +5312,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D34:D35</xm:sqref>
+          <xm:sqref>D30:D31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{F00EA992-7704-4FFF-9390-9F67541314D3}">
@@ -5706,7 +5327,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D15:E16 D2:D23</xm:sqref>
+          <xm:sqref>D11:E12</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{04E5CAC7-3551-4B94-B47C-699E9D4FD15E}">
@@ -5721,7 +5342,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D20:E21</xm:sqref>
+          <xm:sqref>D16:E17</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{0A0C05FE-AFF7-47B4-82C0-19EAEEA3391A}">
@@ -5736,7 +5357,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D22:E23</xm:sqref>
+          <xm:sqref>D18:E19</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{69715B00-4721-4DC7-BD2B-D23473816C64}">
@@ -5751,7 +5372,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D30:E30 E31</xm:sqref>
+          <xm:sqref>D26:E26 E27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{05321CB7-284A-4FA6-BF65-78097A8972CB}">
@@ -5766,7 +5387,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D33:E33 E34:E35</xm:sqref>
+          <xm:sqref>D29:E29 E30:E31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{0F5F82D7-D9D8-496A-8067-873F84F07A41}">
@@ -5781,7 +5402,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D36:E1048576 D1:E1</xm:sqref>
+          <xm:sqref>D32:E1048576 D1:E1</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{98CA02A6-D84B-4B8F-8EE0-BCA3C3E37146}">
@@ -5796,7 +5417,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E12:E14</xm:sqref>
+          <xm:sqref>E8:E10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{2349AB90-2466-4CCB-9A09-AFC1C523F64F}">
@@ -5811,7 +5432,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E17:E19</xm:sqref>
+          <xm:sqref>E13:E15</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{990B53AC-61DA-4898-8173-FDAF9356A9A3}">
@@ -5826,7 +5447,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E24:E26</xm:sqref>
+          <xm:sqref>E20:E22</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{E24EC235-1C22-47A2-9E45-98978623B831}">
@@ -5841,7 +5462,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E27:E28</xm:sqref>
+          <xm:sqref>E23:E24</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{416DB728-3CDE-4A4A-A59B-4A22B9276A40}">
@@ -5856,7 +5477,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E29</xm:sqref>
+          <xm:sqref>E25</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{A7C290DA-E617-4412-A5C5-3335857A068B}">
@@ -5871,7 +5492,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E32</xm:sqref>
+          <xm:sqref>E28</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -6093,7 +5714,7 @@
     </row>
     <row r="2" spans="1:23">
       <c r="A2" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B2" s="41" t="s">
         <v>81</v>
@@ -6162,7 +5783,7 @@
     </row>
     <row r="3" spans="1:23">
       <c r="A3" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B3" s="41" t="s">
         <v>82</v>
@@ -6232,7 +5853,7 @@
     </row>
     <row r="4" spans="1:23">
       <c r="A4" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B4" s="47" t="s">
         <v>83</v>
@@ -6442,7 +6063,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:2">

</xml_diff>

<commit_message>
all working smooth, added some new plots, removed min fraction for gas powerplant, ask seb if ok
</commit_message>
<xml_diff>
--- a/Input/urbs_intertemporal_2050/2024.xlsx
+++ b/Input/urbs_intertemporal_2050/2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxoi\GitHub\urbs-extension\Input\urbs_intertemporal_2050\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6507CB46-1A04-4473-A680-0002A32E6BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0310EB8-B198-46BC-9B5F-FD6C789E7A05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5445" windowWidth="38640" windowHeight="21120" tabRatio="796" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="67080" yWindow="-1935" windowWidth="29040" windowHeight="17520" tabRatio="796" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="11" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="105">
   <si>
     <t>t</t>
   </si>
@@ -2363,7 +2363,25 @@
     <cellStyle name="Zelle überprüfen 4" xfId="214" xr:uid="{00000000-0005-0000-0000-000092010000}"/>
     <cellStyle name="Zelle überprüfen 5" xfId="215" xr:uid="{00000000-0005-0000-0000-000093010000}"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="24">
+    <dxf>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <border>
         <top style="thin">
@@ -3206,7 +3224,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A2:XFD3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -3318,8 +3336,8 @@
       <c r="D5">
         <v>22.68</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>27</v>
+      <c r="E5" s="7">
+        <v>319200000</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>27</v>
@@ -3429,7 +3447,7 @@
   <autoFilter ref="B1:F4" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="B8:B10">
-    <cfRule type="expression" dxfId="21" priority="1">
+    <cfRule type="expression" dxfId="23" priority="1">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3451,7 +3469,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A2:XFD3"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -3629,8 +3647,8 @@
       <c r="E4" s="20">
         <v>0</v>
       </c>
-      <c r="F4" s="63">
-        <v>999999</v>
+      <c r="F4" s="50">
+        <v>53560</v>
       </c>
       <c r="G4" s="52" t="s">
         <v>27</v>
@@ -3676,8 +3694,8 @@
       <c r="E5" s="20">
         <v>0</v>
       </c>
-      <c r="F5" s="63">
-        <v>999999</v>
+      <c r="F5" s="50">
+        <v>43590</v>
       </c>
       <c r="G5" s="52" t="s">
         <v>27</v>
@@ -3715,7 +3733,7 @@
         <v>88</v>
       </c>
       <c r="C6" s="50">
-        <v>188900</v>
+        <v>132230</v>
       </c>
       <c r="D6" s="20">
         <v>9</v>
@@ -3730,7 +3748,7 @@
         <v>27</v>
       </c>
       <c r="H6" s="53">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="I6" s="54">
         <v>802808.92800000007</v>
@@ -3965,7 +3983,7 @@
         <v>27</v>
       </c>
       <c r="H11" s="53">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="I11" s="55">
         <v>1951271.6999999997</v>
@@ -3997,7 +4015,7 @@
         <v>104</v>
       </c>
       <c r="C12" s="50">
-        <v>0</v>
+        <v>56670</v>
       </c>
       <c r="D12" s="20">
         <v>9</v>
@@ -4039,38 +4057,48 @@
   </sheetData>
   <autoFilter ref="A1:N1" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <phoneticPr fontId="0" type="noConversion"/>
-  <conditionalFormatting sqref="A2:A12 B2:B3 D2:E12">
-    <cfRule type="expression" dxfId="20" priority="8">
+  <conditionalFormatting sqref="A1:XFD4">
+    <cfRule type="expression" dxfId="22" priority="12">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD3 A4:E4 G4:XFD4">
-    <cfRule type="expression" dxfId="19" priority="10">
+  <conditionalFormatting sqref="B2:B3 A2:A12 D2:E12">
+    <cfRule type="expression" dxfId="21" priority="10">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B12">
-    <cfRule type="expression" dxfId="18" priority="1">
+    <cfRule type="expression" dxfId="20" priority="3">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="17" priority="3">
+    <cfRule type="expression" dxfId="19" priority="5">
+      <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8">
+    <cfRule type="expression" dxfId="18" priority="7">
+      <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6">
+    <cfRule type="expression" dxfId="17" priority="2">
+      <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11">
+    <cfRule type="expression" dxfId="16" priority="1">
+      <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:K2">
+    <cfRule type="expression" dxfId="15" priority="9">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P9:XFD17 A17 A18:XFD1048576">
-    <cfRule type="expression" dxfId="16" priority="11">
-      <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F8">
-    <cfRule type="expression" dxfId="15" priority="5">
-      <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2:K2">
-    <cfRule type="expression" dxfId="14" priority="7">
+    <cfRule type="expression" dxfId="14" priority="13">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4102,7 +4130,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -4197,8 +4225,9 @@
       <c r="D5" s="24">
         <v>1</v>
       </c>
-      <c r="E5" s="24">
-        <v>1.2</v>
+      <c r="E5" s="24" t="e">
+        <f>D5*E3</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -4232,9 +4261,9 @@
       <c r="D7" s="24">
         <v>0.20499999999999999</v>
       </c>
-      <c r="E7" s="24">
+      <c r="E7" s="24" t="e">
         <f>D7*E5</f>
-        <v>0.24599999999999997</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -4573,8 +4602,9 @@
       <c r="D26" s="24">
         <v>1</v>
       </c>
-      <c r="E26" s="24">
-        <v>1.2</v>
+      <c r="E26" s="24" t="e">
+        <f>D26*E24</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -4668,47 +4698,38 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
-  <conditionalFormatting sqref="A3:C4 E3:XFD4 A5 C5:XFD5 A6:C7 E6:XFD7 A8:XFD12 A13:C15 E13:XFD15 A16:XFD19 F20:XFD28 A30:C31 E30:XFD31 A32:XFD1048576 A1:XFD2 D2:D19">
-    <cfRule type="expression" dxfId="13" priority="34">
+  <conditionalFormatting sqref="A1:XFD2 D2:D19 A3:C4 E3:XFD4 A5 A6:C7 E6:XFD7 A8:XFD12 A13:C15 E13:XFD15 A16:XFD19 F20:XFD28 A30:C31 E30:XFD31 A32:XFD1048576">
+    <cfRule type="expression" dxfId="13" priority="36">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B21:C25 C26:E26 B27:C27">
-    <cfRule type="expression" dxfId="12" priority="20">
+  <conditionalFormatting sqref="B21:C25 C26:D26 B27:C27">
+    <cfRule type="expression" dxfId="12" priority="22">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:D28">
-    <cfRule type="expression" dxfId="11" priority="7">
+    <cfRule type="expression" dxfId="11" priority="9">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:E20 A20:A29 D23:E23">
-    <cfRule type="expression" dxfId="10" priority="21">
+    <cfRule type="expression" dxfId="10" priority="23">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:XFD29">
-    <cfRule type="expression" dxfId="9" priority="1">
+    <cfRule type="expression" dxfId="9" priority="3">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:E2 D2:D19">
-    <cfRule type="dataBar" priority="33">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="2"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{E75D5CC6-8EBE-4E5D-B4DA-5515E5E7F357}</x14:id>
-        </ext>
-      </extLst>
+  <conditionalFormatting sqref="C5:XFD5">
+    <cfRule type="expression" dxfId="8" priority="1">
+      <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:D7">
-    <cfRule type="dataBar" priority="31">
+    <cfRule type="dataBar" priority="33">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -4721,8 +4742,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D10 D5:E5 E3:E4 E6:E7">
-    <cfRule type="dataBar" priority="40">
+  <conditionalFormatting sqref="D8:D10 D5 E3:E4 E6:E7">
+    <cfRule type="dataBar" priority="42">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -4735,8 +4756,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13 D15">
-    <cfRule type="dataBar" priority="29">
+  <conditionalFormatting sqref="D15 D13">
+    <cfRule type="dataBar" priority="31">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -4750,7 +4771,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="dataBar" priority="27">
+    <cfRule type="dataBar" priority="29">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -4764,7 +4785,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20">
-    <cfRule type="dataBar" priority="23">
+    <cfRule type="dataBar" priority="25">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -4778,7 +4799,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22">
-    <cfRule type="dataBar" priority="12">
+    <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -4790,10 +4811,10 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="13">
+    <cfRule type="expression" dxfId="7" priority="15">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
-    <cfRule type="dataBar" priority="14">
+    <cfRule type="dataBar" priority="16">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -4807,7 +4828,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23">
-    <cfRule type="dataBar" priority="22">
+    <cfRule type="dataBar" priority="24">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -4821,7 +4842,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25">
-    <cfRule type="dataBar" priority="9">
+    <cfRule type="dataBar" priority="11">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -4833,10 +4854,10 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="10">
+    <cfRule type="expression" dxfId="6" priority="12">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
-    <cfRule type="dataBar" priority="11">
+    <cfRule type="dataBar" priority="13">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -4850,7 +4871,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28">
-    <cfRule type="dataBar" priority="6">
+    <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -4862,7 +4883,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="dataBar" priority="8">
+    <cfRule type="dataBar" priority="10">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -4876,10 +4897,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29:D31">
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
-    <cfRule type="dataBar" priority="5">
+    <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -4893,7 +4914,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30:D31">
-    <cfRule type="dataBar" priority="3">
+    <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -4906,8 +4927,22 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D2:E2 D2:D19">
+    <cfRule type="dataBar" priority="35">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="2"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{E75D5CC6-8EBE-4E5D-B4DA-5515E5E7F357}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D11:E12">
-    <cfRule type="dataBar" priority="42">
+    <cfRule type="dataBar" priority="44">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -4921,7 +4956,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:E17">
-    <cfRule type="dataBar" priority="36">
+    <cfRule type="dataBar" priority="38">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -4935,7 +4970,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18:E19">
-    <cfRule type="dataBar" priority="35">
+    <cfRule type="dataBar" priority="37">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -4948,22 +4983,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D26:E26 E27">
-    <cfRule type="dataBar" priority="24">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="2"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{69715B00-4721-4DC7-BD2B-D23473816C64}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="D29:E29 E30:E31">
-    <cfRule type="dataBar" priority="4">
+    <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -4977,7 +4998,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:E1048576 D1:E1">
-    <cfRule type="dataBar" priority="61">
+    <cfRule type="dataBar" priority="63">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -4990,8 +5011,22 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="2"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{3721D2A3-FECF-4A8D-8467-880D87B6D2BC}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="E8:E10">
-    <cfRule type="dataBar" priority="39">
+    <cfRule type="dataBar" priority="41">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -5005,7 +5040,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13:E15">
-    <cfRule type="dataBar" priority="37">
+    <cfRule type="dataBar" priority="39">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -5019,7 +5054,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20:E22">
-    <cfRule type="dataBar" priority="26">
+    <cfRule type="dataBar" priority="28">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -5033,12 +5068,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21:E22">
-    <cfRule type="expression" dxfId="5" priority="19">
+    <cfRule type="expression" dxfId="4" priority="21">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:E24">
-    <cfRule type="dataBar" priority="25">
+    <cfRule type="dataBar" priority="27">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -5051,13 +5086,13 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E24:E25">
-    <cfRule type="expression" dxfId="4" priority="17">
+  <conditionalFormatting sqref="E24:E28">
+    <cfRule type="expression" dxfId="3" priority="17">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="dataBar" priority="18">
+  <conditionalFormatting sqref="E25:E26">
+    <cfRule type="dataBar" priority="20">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -5070,13 +5105,22 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E27:E28">
-    <cfRule type="expression" dxfId="3" priority="15">
-      <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
+  <conditionalFormatting sqref="E27 D26">
+    <cfRule type="dataBar" priority="26">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="2"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{69715B00-4721-4DC7-BD2B-D23473816C64}</x14:id>
+        </ext>
+      </extLst>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28">
-    <cfRule type="dataBar" priority="16">
+    <cfRule type="dataBar" priority="18">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -5098,21 +5142,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{E75D5CC6-8EBE-4E5D-B4DA-5515E5E7F357}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>2</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>D2:E2 D2:D19</xm:sqref>
-        </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C0F1B5C9-46CC-4068-A4A5-2BE845D64618}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
@@ -5141,7 +5170,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D8:D10 D5:E5 E3:E4 E6:E7</xm:sqref>
+          <xm:sqref>D8:D10 D5 E3:E4 E6:E7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{FD70C683-63D2-4AF7-9844-0053BE6DF679}">
@@ -5156,7 +5185,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D13 D15</xm:sqref>
+          <xm:sqref>D15 D13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C12684E9-C44A-443A-881A-7ED428CB9718}">
@@ -5315,6 +5344,21 @@
           <xm:sqref>D30:D31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{E75D5CC6-8EBE-4E5D-B4DA-5515E5E7F357}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D2:E2 D2:D19</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{F00EA992-7704-4FFF-9390-9F67541314D3}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
@@ -5360,21 +5404,6 @@
           <xm:sqref>D18:E19</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{69715B00-4721-4DC7-BD2B-D23473816C64}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>2</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>D26:E26 E27</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{05321CB7-284A-4FA6-BF65-78097A8972CB}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
@@ -5403,6 +5432,21 @@
             </x14:dataBar>
           </x14:cfRule>
           <xm:sqref>D32:E1048576 D1:E1</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{3721D2A3-FECF-4A8D-8467-880D87B6D2BC}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{98CA02A6-D84B-4B8F-8EE0-BCA3C3E37146}">
@@ -5477,7 +5521,22 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E25</xm:sqref>
+          <xm:sqref>E25:E26</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{69715B00-4721-4DC7-BD2B-D23473816C64}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E27 D26</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{A7C290DA-E617-4412-A5C5-3335857A068B}">

</xml_diff>